<commit_message>
Feat: constant for multiple Uni
</commit_message>
<xml_diff>
--- a/data/ED/program_details_sample.xlsx
+++ b/data/ED/program_details_sample.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD4"/>
+  <dimension ref="A1:BD11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,115 +704,111 @@
       </c>
     </row>
     <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>University College London</t>
+          <t>The University of Edinburgh</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>伦敦大学学院</t>
+          <t>爱丁堡大学</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>School: Edinburgh College of Art | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Msc Acoustics And Music Technology</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Taking the science of sound as your focus, you’ll work in a cross-disciplinary environment. You will use theoretical and experimental work to explore the musical, technical and multimedia applications of acoustics and audio technology.
+The emphasis of this programme is on science and technology in the context of musical and multimedia applications.
+The programme aims to:
+provide a broadly based, scientifically-oriented foundation in the area of acoustics, audio, and music technology
+develop your skills in research, computation, design and analytical problem-solving
+give you a strong understanding of music/audio technology
+create a multidisciplinary learning environment that will prepare you for a future career
+You can find more information on the Acoustics and Audio Group website.
+MSc in Acoustics and Music Technology</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Teaching
+The MSc is taught by a combination of:
+Lectures
+Seminars
+Assessment and dissertation
+Courses are assessed through a combination of report submissions and written examinations.
+In the final three months of the programme, you will carry out an individual project. This is assessed by the submission of a dissertation.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>- Lectures
+ - Seminars
+ - Tutorials 
+ - practical work</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=478</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>two years. In the final three months of the programme, you will carry out an individual project. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>This programme, developed in partnership with the NHS, combines academic
-teaching with clinical practice training in applied psychology for children
-and young people.
-It allows you to develop knowledge and competence in the delivery of evidence-based psychological interventions for this group, and skills and competencies for the delivery of Tier two psychological assessments and interventions in services for children, young people and their families.
-You will be employed in a one-year clinical placement in the Scottish NHS Child &amp; Adolescent Mental Health Service, gaining valuable experience applying psychological theory to
-practice, under the supervision of a qualified clinical psychologist.
-Alongside
-essential elements for applied psychologists in health (e.g. assessment
-and formulation, and evaluation) and child and adolescent mental health
-professionals (e.g. safeguarding children, child and adolescent development
-and health promotion), there is a particular focus on psychological interventions, early years and early
-intervention. There is also a strong emphasis on parenting and supporting
-parents through evidence-based models of parent-focused intervention.
-The clinical experience gained on placement facilitates linking theory to practice and fosters the development of professional skills necessary for post-qualification practice.</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>The programme is a one year, full-time course with teaching delivered at both the University of Edinburgh and NHS partnership sites in Glasgow.
-Clinical placements will be with one of the NHS Health Boards within Scotland.
-Courses include:</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>- Assessment and Formulation
- - Child and Adolescent Development
- - Early Years and Early Intervention
- - Evaluation and Research
- - Professional Context and Clinical Management
- - Promotion of Mental Health and Emotional Wellbeing
- - Psychological Intervention and Structured Treatment Approaches</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=129</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Start date: February Awards: MSc (12 mth FT).</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>信息不可用 Tuition Fees找不到</t>
-        </is>
-      </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>信息未找到</t>
+          <t>Academic: total 7.0 with at least 6.0 in each component.</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>需要</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>you will be required to attend an interview as part of our selection process.</t>
+          <t>未要求</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>未要求</t>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>if you do not meet the academic entry requirements, we may still consider your application if you have professional experience.</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
@@ -822,99 +818,971 @@
       </c>
     </row>
     <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>University College London</t>
+          <t>The University of Edinburgh</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>伦敦大学学院</t>
+          <t>爱丁堡大学</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>School: Engineering | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Msc Advanced Chemical Engineering</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>From carbon capture to sustainable water resources, from alternative energy technologies to advanced pharmaceutical processes, chemical engineers address the frontiers of important global challenges. They formulate and solve today the design problems for the technologies of tomorrow.
+This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields.
+You will learn through:
+taught modules
+coursework
+design projects
+guest lectures
+workshops
+an MSc Research Dissertation
+a number of career supporting activities
+This programme has a particular emphasis on multi-scale approaches and integrated solutions to chemical engineering problems, from the nano-scale to the process scale.
+Learn from industry specialists
+A unique feature of our MSc programme in Advanced Chemical Engineering (ACE) is the strong and committed involvement of the UK and EU chemical engineering industry.
+The programme is advised by an Industrial Advisory Board, and all our MSc Research Dissertation projects are formulated and co-advised by industrial partners, with a wide range of topics including:
+novel processes and materials for carbon capture and storage against climate change
+innovative solutions for energy storage and fuels
+efficient process systems for pharmaceuticals, food and drink manufacturing
+modern concepts and prototypes in healthcare, biomedicine and biotechnology
+Our MSc programme attracts a huge diversity of talent, with 60+ graduates and current students from over 20 countries, spanning four continents. We also work with over 40 industrial partners who help develop and supervise our MSc Research Dissertation projects, ensuring these reflect the latest industry trends and challenges.
+Accreditation
+Accreditation of this MSc for CEng (Further Learning) means that our graduates who are seeking to become Chartered Engineers can count their MSc in Advanced Chemical Engineering as one year of Further Learning when applying for the Chartered Engineer status.
+The CEng accreditation is awarded by the Institution of Chemical Engineers (IChemE), which is an independent professional body. It gives students and employers confidence in the quality of the MSc Advanced Chemical Engineering programme.</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>In Semester 1, the MSc ACE programme establishes a foundation through compulsory courses which emphasise modern computational techniques and research methods.
+In Semester 2, you will expand your knowledge through a broader selection of optional courses. These focus on:
+A minimum of 10 credits must come from a subset of three Advanced Design optional courses.
+You will have the unique opportunity to:
+Students must select at least one of the next three courses:
+Students can select one of the following courses during Semester 1:
+Plus, between three and six of the following courses (depending on above Advanced Design choices, for a total of 120 credits) during Semester 2:
+The Advanced Chemical Engineering Dissertation (MSc) follows early project allocation and substantial training during Semesters 1-2.
+After the completion of taught modules and confirmation of progression, students focus exclusively on their research project during Semester 3, under the joint supervision of an academic and an industrial partner, with several feedback opportunities.</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>- energy-efficient separation processes
+ - multidisciplinary engineering
+ - management and economics
+ - several cutting-edge technological fields
+ - learn from leading experts in several fields
+ - explore actual industrial processes (with emphasis on design and energy efficiency)
+ - acquire technical skills in various areas
+ - implement them to actual chemical engineering problems
+ - hone your communication and human skills to present your original achievements
+ - Numerical Methods for Chemical Engineers
+ - Molecular Thermodynamics 
+ - Introduction to Research Methods 
+ - Advanced Chemical Engineering Dissertation
+ - Separation Processes for Carbon Capture (Semester 2)
+ - Oil and Gas Systems Engineering (Semester 2)
+ - Group Design Project (Advanced Chemical Engineering Design) (Semester 2)
+ - Chemical Reaction Engineering 
+ - Fire Science and Fire Dynamics
+ - Engineering Project Management 
+ - Supply Chain Management  
+ - Technology and Innovation Management 
+ - Technology Entrepreneurship
+ - Adsorption
+ - Gas Separations Using Membranes 
+ - Separation Processes
+ - Advanced Process Safety
+ - Batchwise and Semibatch Processing 
+ - Bio-Inspired Engineering 
+ - Biotechnology and Bioprocess Engineering
+ - Polymer Science and Engineering
+ - Nanomaterials in Chemical and Biomedical Engineering 
+ - Electrochemical Engineering 
+ - Particle Technology Fundamentals and Industrial Applications</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=913</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>one-year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Accreditation of this MSc for CEng (Further Learning) means that our graduates who are seeking to become Chartered Engineers can count their MSc in Advanced Chemical Engineering as one year of Further Learning when applying for the Chartered Engineer status. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields.</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>School: Informatics | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Msc Advanced Technology For Financial Computing</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>This programme will provide you with a critical and practical appreciation of how data, computing and artificial intelligence technologies can be used and developed. You will learn how this deliver value in organisations with finance, risk and decision-making related digitalisation from both technology and business perspectives.
+The move towards digital organisations offers great potential for small and large, public and private enterprises. Edinburgh is in the UK's second largest financial centre after London and is leading cutting-edge, data-driven innovation to become the data capital of Europe.
+This programme is taught by world class researchers and educators. It is based on full-time cross-disciplinary study and has strong links to existing centres of research excellence within three world-class academic schools within the University:
+School of Informatics
+Edinburgh Business School
+School of Mathematics</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work. This leads to a dissertation focused on both academic and real-world industry challenges.
+It provides a unique blend of advanced technical courses, including finance-related sectors, and digital business skills with an emphasis on finance elements (minimum 30 credits) from Edinburgh Business School.
+The programme provides you with unique interdisciplinary training. Computing courses build your technical skills. Maths and finance related courses develop your ability to understand the finance system challenges associated with the development, implementation and exploitation of technical solutions.</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=992</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work.</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Academic: total 7.0 with at least 6.5 in each component.</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>School: Engineering | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Msc Advanced Power Engineering</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:
+taught modules
+workshops
+a comprehensive research dissertation carried out during the second year of the programme
+support from the internationally-leading experts of the Institute for Energy Systems
+Our academics regularly lead or participate in large, multi-institutional and multi-national research projects in the area of electrical power engineering. The learning experience is augmented by a number of supporting activities delivered throughout the duration of the programme.
+How will I learn?
+Graduates will be equipped with specialised knowledge associated with the individual modules within the programme. You will develop a deep understanding of advanced power engineering concepts fostered throughout the programme and obtained from the supplementary training activities, study projects and the 2nd year research project.
+The first year of the programme develops from fundamental topics and research tools and techniques in electrical power engineering, to specialist courses on emerging technologies and advanced numerical methods for power engineering problems.
+Research project
+Following the summer break, the second year of the programme is fully dedicated to the Masters research project.
+In close collaboration with academics and researchers of the Institute for Energy Systems, you will put into practice the knowledge and skills acquired during the first year, in application to an actual power engineering problem.
+For the research project there is an option to carry it out within either:
+one of our power research groups, working alongside academics and researchers of the Institute for Energy Systems
+an industrial placement at a collaborating company in the power sector
+Accreditation
+The MSc in Advanced Power Engineering has been accredited by the UK Institution of Engineering and Technology (IET), one the largest professional engineering bodies in the world.
+Your MSc in Advanced Power Engineering can therefore count against the academic requirements for registration as a Chartered Engineer (CEng) in the UK.
+Chartered Engineers not only have a firm grasp of the underpinning knowledge of their field, but also possess the required professional skills to excel in the modern engineering environment.
+Accredited programmes undergo continuous and robust quality review by the IET, and are internationally recognised for their quality of the education they provide.</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>The programme is delivered over 2 years. In Year 1 there are two semesters of taught courses; in Year 2 a research project runs over two semesters leading to the submission of a masters thesis.
+The courses correspond to 120 credits of taught material, plus 120 credits of a research project.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>- Distributed Energy Resources and Smart Grids
+ - Power Engineering Fundamentals 
+ - Power Engineering Laboratory 
+ - Engineering Research Methods with Grand Challenge
+ - Power Systems Engineering and Economics 
+ - Principles of Wind Energy 
+ - Solar Energy &amp; Photovoltaic Systems 
+ - Advanced Power Electronics and Machines 
+ - Research Project: Advanced Power Engineering Dissertation</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=960</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>two-year. The programme is delivered over 2 years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>this requirement may be partially met by relevant industrial experience; applicants with non-standard backgrounds may be considered on a case-by-case basis.</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>School: Social &amp; Political Science | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Master's Advanced Social Work Studies (mental Health Officer Award) Pgcert</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>This programme is the postgraduate qualification for qualified social workers wishing to practice as mental health officers (MHOs). It has been designed and delivered in partnership with 13 local authorities in the East of Scotland and the University of Edinburgh.
+The programme focuses upon the role of the MHO in relation to relevant Scottish legislation.
+Under Section 32(2) of the Mental Health (Care and Treatment) (Scotland) Act 2003 (the 2003 Act), local authorities have a statutory duty to appoint MHOs to undertake mandatory responsibilities, enshrined in legislation, currently:
+the 2003 Act
+the Adults with Incapacity (Scotland) Act 2000
+the Criminal Procedures (Scotland) Act 1995
+The programme also prepares MHOs to integrate knowledge of other relevant legislation, including:
+the Adult Support and Protection (Scotland) Act 2007
+Its primary aim is to provide the Advanced Social Work Studies (Mental Health Officer Award) in partnership with the East of Scotland MHO Award Partnership.</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>The programme comprises four courses and two practice placements which are taught over one academic year.
+We start with two days induction in mid-October followed by the first course, which begins in late November/December.
+It provides an introduction to some of the key issues and current thinking in the field of mental health and encourages students to take a critical look at subjects and concepts including mental illness, psychiatric diagnoses, recovery and contemporary developments in mental health law.
+The subsequent three courses are structured around the main statutes that frame the MHO role, namely:
+Teaching and learning activities enable students to gain a detailed understanding of this framework and how it interfaces with adult protection legislation.
+The programme benefits from inputs from practising MHOs and allied professionals, including psychiatrists, psychologists and advocacy workers.
+A central focus is the pivotal role MHOs play in navigating the ethical and human rights challenges inherent in this work. This is supported by contributions from people with experience of mental distress and their carers.
+The programme structure enables students to apply their academic learning to real-life situations during the practice placements, supported and supervised by experienced MHOs.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>- The Mental Health (Care and Treatment) (Scotland) Act 2003
+ - The Criminal Procedures (Scotland) Act 1995
+ - The Adults with Incapacity (Scotland) Act 2000</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=634</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. A UK 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>Academic: total 7.0 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>a uk 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice.</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>School: Edinburgh College of Art | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Msc Advanced Sustainable Design</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Advanced Sustainable Design gives you the knowledge, skills and creativity to put theory into practice in the sustainable development of our cities, towns and countryside. We work from the scale of building systems to entire regions.
+We welcome applications from graduates of all disciplines. This programme engages with architecture, design and planning but interested applicants can apply with degrees in the environmental sciences and the humanities.
+Our programme is delivered in a series of practical projects supplemented with teaching on all aspects of built environment sustainable design. You will have the opportunity to work in building simulation modelling and gain desirable skills for the workplace.
+We believe that successful sustainable development is not achieved only through technical solutions. You will:
+explore the complex relationship of design to contemporary sustainable agenda
+engage in cultural and professional debates about the built environment
+gain a distinctive and expert voice in this field
+This programme is affiliated with the University’s Global Environment &amp; Society Academy:
+Global Environment &amp; Society Academy</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>You will complete your studies in one year.
+The first semester is a combination of theory and practice. We will explore the theoretical underpinnings of sustainable design, from a planetary scale to that of a building component.
+Alongside this, you will work on design projects at the scale of both settlements and building systems. We set many of our projects on a global stage, working in a range of climates and contexts.
+The second semester offers an immersive design project that allows you to make your own projects and test them in real contexts.
+You will conclude your studies with a comprehensive dissertation research project that can advance your own interests and be shaped to your preferred career path.</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=417</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>one year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. You will complete your studies in one year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>your portfolio should be one, single pdf file of no more than 10 pages. if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Msc Advanced Nursing</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>This innovative programme offers advanced study for nurses working within a global context to enhance practice at the local level.
+You can either choose a specific pathway: leadership, clinical research* or education, or follow a flexible generic programme with the opportunity to study a range of relevant courses from across the School of Health in Social Science and the wider University.
+Nursing, health and social care research underpins the whole programme.
+You will begin the MSc at the same entry point as all other students, but depending on the pathway you would like to undertake, have the opportunity to exit with a range of different degree titles:
+MSc Advanced Nursing
+MSc Advanced Nursing (leadership)
+MSc Advanced Nursing (education)
+MSc Advanced Nursing (clinical research)
+Who is this programme for?
+The programme is suitable if you are a nurse registered in any branch of the profession to practice in your own country and you want to critically examine the ways that evidence-based research, theory and knowledge can advance nursing in the global context.
+The degree also provides an excellent foundation for postgraduate research e.g. a doctoral degree, or to advance their professional career.
+*The clinical research pathway is only available for students who are registered with the Nursing Midwifery Council in the UK to practice in a clinical setting.</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Teaching is delivered in a range of engaging and interactive formats by academic and specialist staff working in the contemporary health care environment.
+Teaching methods include:
+As a full-time MSc student, you will take two core courses and two option courses each semester.
+There is a choice of one of three different dissertations:
+This is to be completed during the Semester 3.
+You can follow one of three different pathways: leadership, education or clinical research, or can take a generic pathway, depending on career aspirations and areas of interest.
+As a part-time student, you can choose one or two courses each semester and have a choice of dissertation in your final year.
+You can also follow the three different pathways or take a generic pathway.
+The compulsory courses form the core part of the MSc and are:
+You can then choose 4 optional taught courses before you go on to undertake the dissertation.
+Optional courses can be chosen from those on offer within the School of Health in Social Science or across the wider University and are dependent on the pathway that the student chooses.
+Optional courses vary across years depending on the specific courses on offer, but some of the current optional courses available include:</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>- lectures
+ - seminars
+ - workshops
+ - tutor-led online learning environments
+ - empirical
+ - research proposal
+ - e-portfolio
+ - Global Leadership in Nursing: Policy, Informatics and Innovation
+ - Designing research in Nursing, Health and Social care
+ - Clinical Decision Making and Professional Judgement
+Teaching Practice Attachment
+ - Leadership - exploring your potential (distance)
+ - Global Public Health: a critical approach to health improvement
+ - Conducting Research in Nursing, Health and Social care
+ - Health Research Methods workshops
+ - Homeless and Inclusion Health
+ - Cancer Care
+ - Transplant nursing
+ - Community nursing
+ - Person Centred Care in Practice: Relationships and Emotion</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=419</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Msc Online Advanced Nursing (online Learning)</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Our innovative part-time programme offers advanced study for nurses working within an international and UK health care context. 
+We offer the flexibility for you to choose either a broad programme of study by drawing on international expertise across the breadth of the university, or to focus on a more specialised area of nursing care.
+We recognise that mental health and trauma-informed care is an under-developed area in advanced practice for Adult nurses and so we are delighted to offer you the opportunity to choose option courses in these areas, as well as our core courses in nursing and global health policy, political leadership and research. 
+You can choose a range of option courses within Nursing Studies including leadership, public health, policy, person-centred care and clinical decision making. Health and social care research underpin the whole programme.
+The programme is suitable for nurses who are registered to practise in their own country and want to critically examine the ways that evidence-based research, theory and knowledge can advance nursing in the global context. The degree also provides an excellent foundation for postgraduate research e.g. a doctoral degree, or to advance their professional career.</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>This programme offers a flexible online postgraduate degree designed for graduate nurses who are interested in studying at an advanced level.
+The programme is designed to be completed part-time. The minimum period the programme can be completed is two years, with a maximum completion time of three years.
+Students must take two core courses (40 credits) and then can choose from a wide range of option courses offered in semesters 1 and 2 (80 credits). Supervised Reading is also offered in the summer semester (20 credits). In addition, students must complete a dissertation following completion of their taught courses (60 credits). There is a choice of one of two different dissertations – research proposal or e-portfolio.
+For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2. Their dissertation will be completed towards the end of their second year.
+For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. Their dissertation will be completed in year 3.
+The compulsory courses form the core part of the MSc are:
+Optional courses can be chosen from those on offer within the School of Health in Social Science or across the wider university. These vary across years depending on the specific courses on offer, but some of the current nursing online optional courses include:
+We are also delighted to offer a range of option courses with our colleagues in Clinical Psychology and Counselling and Psychological Therapies. 
+This enables you to learn from our team of international experts to inform advanced nursing practice in relation to mental health and trauma-focused health care.
+These option courses include:
+For the latest information available, please see the DRPS.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>- Nursing and Global Health Policy: developing your political leadership
+ - Research Methods in Health
+ - Leadership – exploring your potential
+ - Global Public Health: a critical approach to health improvement
+ - Person Centred Care in Practice: relationships and emotion
+ - Supervised Reading
+ - Online Counselling Practice and Process
+ - Developmental Wellbeing
+ - Social Inequality and Child and Adolescent Mental Health
+ - Applied Developmental Psychology
+ - Trauma and Resilience in a Developmental Context</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=1049</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>two years. MSc Advanced Nursing (Online Learning) (ICL) - 2-6 years (Part-time Intermittent Study) Select your start date 11 September 2023. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. The minimum period the programme can be completed is two years, with a maximum completion time of three years. For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Tuition fees Award Title Duration Study mode   MSc Advanced Nursing Up to 6 Years Part-time Intermittent Study Tuition fees. For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2.</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>Fees for part-time intermittent study
+If you are studying on a part-time intermittent basis then you will be invoiced separately for each course. We refer to this as Invoiced at Course Level (ICL).
+The fees you will pay depend on whether your degree takes place online or on campus.
+Online learning: fees for ICL/intermittent degrees
+On-campus: fees for ICL/intermittent degrees
+Annual tuition fee increase
+Tuition fees increase every year in the majority of cases.
+For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
+From 2023-24 tuition fees for new entrants will be fixed for the duration of their programme. If you joined us from August 2023 onwards and you are studying for a degree or qualification that will take more than one year to complete, the fee charged will be fixed at the level charged on the year of entry.
+Fees and funding
+Work out your fee status
+Find out how and when to pay your tuition fees
+Search for scholarships and funding</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>Academic: total 7.0 with at least 6.5 in each component.</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>School: Business School | College: Arts, Humanities &amp; Social Sciences</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Msc Accounting And Finance</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>The full-time MBA is an intensive programme designed for students with a minimum of three years' managerial experience who wish to progress to more senior and leadership roles in business.
-The programme immerses students in a world of academic thought, current business practice and applied projects.
-Studied over 12 months, this is a taught programme delivered by world class faculty complemented by guest business practitioners.
-Successful businesses in the future will be those that can confidently and capably steer a path through a world characterised by intense competition, rapid technological development, economic turbulence and increasing resource insecurity.
-Businesses need leaders who can think and act strategically in this volatile environment, managing the risk and challenges involved, but also spotting and seizing opportunities for efficiency, innovation and new business models. Businesses also need leaders who will act responsibly in delivering value to all stakeholders.
-Our programme enhances your career potential by giving you a clear focus on the role of the highly sought strategic leader and helps you to progress with confidence. In order to achieve this our MBA is built on three pillars:
-Strategic Leadership
-Professional Development
-Personalised Approach</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>The MBA is delivered full-time starting in September each year. The programme combines intensive academic study with practical application. This is achieved both in the classroom through case studies, but also via consultancy-style projects with external organisations to broaden participants’ insights into alternative business models and approaches.
-The MBA programme includes a number of compulsory courses as well as a range of specialist courses for you to choose from. For the Edinburgh MBA we have also fully immersed our Professional Development programme into the curriculum as we recognise the value it delivers to our participants. Your studies will culminate in a major Capstone Project.
-For those who want an international experience, there is an opportunity to study on our MBA (with international exchange) which will give you the chance to spend 2-3 months on an exchange at one of our international partner Universities (Australia, Canada, China, Finland, France, Mexico, Spain and USA).
-The programme is delivered in four parts:
-June–August: students undertake a Capstone Project as the final part of the 12-month MBA
-Details of programme structure and elective courses
-The MBA (with International Exchange) programme is delivered in four parts:
-June–August: students undertake a Capstone Project as the final part of the 12-month MBA.
-Details of programme structure and elective courses
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Our Accounting and Finance MSc is closely in line with professional practice and is an ideal fit if you are from a quantitative background.
+This is a programme that will challenge you academically, and, through practical applications and case studies, one that will set you up for future roles within Accounting and Finance.
+Industry connections
+Studying accounting and finance in Edinburgh will give you the opportunity to be based at the heart of the UK's second largest financial centre. Many of Europe's leading financial institutions have their headquarters here, a fact that we make full use of on the MSc programme.
+We regularly bring guest speakers to the School to talk directly to Accounting and Finance students on real, current practice.
+The School also maintains good relationships with a number of accounting and finance professionals who will be on hand to provide advice on research and career opportunities. Essential connections like these characterise the dynamic nature of this programme.
+Our strong connection to industry is exemplified by our work in the Centre for Financial Markets Research, and the Institute of Public Sector Accounting Research.
+Bringing together leading academics and practitioners, the centres are a keen theatre of debate, creating new thoughts, new ideas for both the theoretical study and practical application of accounting, finance and investment.</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Learning will primarily be through:
+Assessment methods include examinations, assignments, presentations or continuous assessment.
 We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>- September–December: students focus on core business disciplines
- - January–March: students develop integrative and strategic thinking, and choose a number of specialist elective subjects
- - April–June: students' specialisation continues
- - June–August: students undertake a Capstone Project as the final part of the 12-month MBA
- - Details of programme structure and elective courses
- - September–March: students study the same core disciplines, integrating courses and a number of specialisations as the main MBA programme
- - April–June: students study abroad at one of 9 partner institutions worldwide, experiencing new cultures and new ways of business
- - June–August: students undertake a Capstone Project as the final part of the 12-month MBA.
- - Details of programme structure and elective courses</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=267</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Studied over 12 months, this is a taught programme delivered by world class faculty complemented by guest business practitioners. For those who want an international experience, there is an opportunity to study on our MBA (with international exchange) which will give you the chance to spend 2-3 months on an exchange at one of our international partner Universities (Australia, Canada, China, Finland, France, Mexico, Spain and USA). MBA Business Administration - 1 Year (Full-time)Select your start date9 September 2024MBA Business Administration with International Exchange - 1 Year (Full-time)Select your start date9 September 2024.</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>- lectures
+ - set reading
+ - class discussions
+ - exercises
+ - group-work assignments
+ - problem-solving in tutorials 
+ - case studies
+ - MSc Accounting and Finance programme structure overview</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=416</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>two years. Tuition fees Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Tuition fees. MSc Accounting and Finance - 1 Year (Full-time) Select your start date 9 September 2024. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Programme structure 2023/24.</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>Programme fees: Business Administration (MBA) (Full-time) - 12 Months
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>Programme fees: Accounting and Finance (MSc)
 Academic Session
 Scotland
 Rest of
@@ -926,7 +1794,7 @@
 2024/5
 Home fees have still to be agreed
 Home fees have still to be agreed
-£40,900.00
+£39,500.00
 Annual tuition fee increase
 Tuition fees increase every year in the majority of cases.
 For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
@@ -937,168 +1805,139 @@
 Search for scholarships and funding</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>信息未找到</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>需要</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>before applying for the full-time mba programme, please consider our minimum entry requirements, which include academic qualifications, managerial work experience and english language requirements. *important points to note when applying for this programme at least three years' work experience in a managerial role. before applying for the full-time mba programme, please consider our minimum entry requirements, which include academic qualifications, managerial work experience and english language requirements. *important points to note when applying for this programme at least three years' work experience in a managerial role.</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>Academic: total 7.0 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
         <is>
           <t>未要求</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>University College London</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>伦敦大学学院</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>School: Royal (Dick) School of Veterinary Studies | College: Medicine &amp; Veterinary Medicine</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Master's Online Advanced Clinical Practice (online Learning) Pgprofdev</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Veterinary medicine is a rapidly evolving discipline, comprising a wide range of specialist areas. Research in veterinary medicine is directly relevant to the improvement of health and welfare of domestic animal species and the protection of public health.
+Research reputation
+The R(D)SVS has an international reputation, and its clinical services - Hospital for Small Animals (dog and cat and exotics, zoo and wildlife) and Large Animal Hospital (equine and livestock) - are among the most influential centres for clinical care in the UK and Europe. It is best placed to advance the skills of the sector due to the skills in primary, secondary and tertiary care medicine and surgery, and its extensive research activities in all aspects of veterinary medicine.
+Who is this programme for?
+Veterinary practitioners are under pressure to maintain high standards of practice while also keeping abreast of the latest developments. In response to the increasing requirement for support in developing advanced clinical skills, this distance learning programme is aimed primarily, but not exclusively, at veterinarians in practice.
+How will I learn?
+The modular, portfolio approach allows the greatest flexibility to meet the needs of the modern practitioner. The goal is to provide you with the skills and knowledge required to be a highly effective practitioner and to enable you to act as a leader and mentor within the veterinary community.</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci.
+In summary, the completion times are as follows:
+The programme is modular in structure, offering a flexible student-centred approach to the choice of courses studied. You can choose to take a particular species track in the elective course, i.e. courses focussed on companion animals, exotic zoo and wildlife, equine or production animals. Equally, you can choose to take a mixed-practice approach by selecting courses that meet your individual professional needs.
+Each year will consist of three 11-week terms structured into two blocks of five weeks of study with a week in between for independent study and reflection. One block of five weeks will equate to 10 credits of course material. This framework is designed to fit in with the part-time nature of the programme, giving you time to reflect on your learning and lessening the impact of the additional requirements that studying will place on your working life.
+Postgraduate Professional Development (PPD) is aimed at working professionals who want to advance their knowledge through a postgraduate-level course(s), without the time or financial commitment of a full Masters, Postgraduate Diploma or Postgraduate Certificate.
+You may take a maximum of 50 credits worth of courses over two years through our PPD scheme. These lead to a University of Edinburgh postgraduate award of academic credit. Alternatively, after one year of taking courses you can choose to transfer your credits and continue on to studying towards a higher award on a Masters, Postgraduate Diploma or Postgraduate Certificate programme. Although PPD courses have various start dates throughout a year you may only start a Masters, Postgraduate Diploma or Postgraduate Certificate programme in the month of September. Any time spent studying PPD will be deducted from the amount of time you will have left to complete a Masters, Postgraduate Diploma or Postgraduate Certificate programme.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>- PgCert: 12-24 months
+ - PgDip: 24-48 months
+ - MVetSci: 36-72 months
+ - More information on PPD</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=910</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>three years. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci. Alternatively, after one year of taking courses you can choose to transfer your credits and continue on to studying towards a higher award on a Masters, Postgraduate Diploma or Postgraduate Certificate programme. The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. Tuition fees Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Tuition fees. PG Professional Development Advanced Clinical Practice (Online Learning) (ICL) - 1-2 Years (Part-time Intermittent Study) Select your start date 11 September 2023 8 January 2024 1 April 2024. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. You may take a maximum of 50 credits worth of courses over two years through our PPD scheme. Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Programme structure 2023/24.</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>School: Education and Sport (Moray House) | College: Arts, Humanities &amp; Social Sciences</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>This two-year Masters programme is for graduates who want a teaching qualification designed to make an explicit difference to the lives of children and young people: it will support you in becoming a beginning teacher with a transformative orientation.
-The MSc in Transformative Learning and Teaching programme provides an in-depth and integrated learning experience, with time spent in both University and school sites throughout the two years, allowing you to develop your skills as a beginning teacher over a longer period of time than would be the case in a Professional Graduate Diploma in Education (PGDE) programme. You will also graduate from this programme with a full masters degree, something that is increasingly seen as desirable for the Scottish teacher workforce as a whole, together with a teaching qualification which will allow you to work across the primary/secondary transition.
-This programme is future-oriented, drawing on cutting-edge research, and is designed to prepare new teachers for a career in teaching in an ever-changing world. It has a particular focus on:
-social justice
-sustainability
-global perspectives
-digital and statistical literacy
-professional inquiry skills
-Pathways
-The programme has a central focus on transformative practice, and, uniquely, will entitle graduates to teach across the primary/secondary transition phase. You will be able to choose from one of the following pathways:
-Nursery - Secondary 3 Pathway
-Primary 5 - Secondary 6 Pathway in a specific subject. Subject specialisms offered are: Computing Science, English, Languages, and Mathematics.*
-Mental health and wellbeing partnership
-Student teachers at the University of Edinburgh also engage with our mental health and wellbeing programme.
-This is provided through our unique partnership with children’s mental health charity Place2Be and helps you to support mental wellbeing in your classrooms and in yourself.
-Place2Be at Moray House
-Accreditation
-Graduates are qualified to teach and eligible for provisional registration from the General Teaching Council for Scotland (GTCS). Eligible graduates may join the Teacher Induction Scheme, a guaranteed, paid one-year probationary teaching post, or take up a Flexible Route.
-This programme is subject to reaccreditation with the General Teaching Council for Scotland (GTCS) in 2023.</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Throughout the duration of the programme, students will engage in both university-based learning and site-based learning in schools, with groups of students being placed in school clusters: one cluster in Year 1 and a different cluster in Year 2.
-A cluster will typically be one secondary school together with associated primary and nursery provision. Placing you in groups will facilitate collaborative learning and support.
-Compulsory courses include:
-In Year 2 of the programme, all students choose 40 credits made up of one 20 credit Digital Education course and one 20 credit Outdoor Environmental Education course.
-We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>- Assessing what matters
- - Children and young people
- - Developing teacher professionalism
- - Literacy, learners and learning
- - Numeracy, learners and learning
- - Teacher literacies
- - Understanding the nature of knowledge and curriculum
- - Your subject specialism</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=938</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>MSc Transformative Learning and Teaching (Nursery S3, Generalist) - 21 Months (Full-time)Select your start date11 September 2023MSc Transformative Learning and Teaching (P5 S6, Computing Science) - 21 Months (Full-time)Select your start date11 September 2023MSc Transformative Learning and Teaching (P5 S6, English) - 21 Months (Full-time)Select your start date11 September 2023MSc Transformative Learning and Teaching (P5 S6, Mathematics) - 21 Months (Full-time)Select your start date11 September 2023MSc Transformative Learning and Teaching (P5 - S6, Languages) - 21 Months (Full-time)Select your start date11 September 2023.</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Tuition Fee: Transformative Learning and Teaching (Nursery - S3, Generalist) (MSc) - 21 Months
-Fees for this degree programme are on the Tuition Fees website.
-Transformative Learning and Teaching fees
-Annual tuition fee increase
-Tuition fees increase every year in the majority of cases.
-For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
-From 2023-24 tuition fees for new entrants will be fixed for the duration of their programme. If you joined us from August 2023 onwards and you are studying for a degree or qualification that will take more than one year to complete, the fee charged will be fixed at the level charged on the year of entry.
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>If your fees do not display, please check the Tuition Fees website and check your fees by level and year of study.
+Find your tuition fees
 Fees and funding
 Work out your fee status
 Find out how and when to pay your tuition fees
 Search for scholarships and funding</t>
         </is>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>信息未找到</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>需要</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>selection involves a professional interview.</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>加分项</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>we may also consider your application if you have other academic or professional qualifications or considerable relevant experience; please contact us to check before you apply.</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
         <is>
           <t>未要求</t>
         </is>

</xml_diff>

<commit_message>
Fix ED IELTS Format
</commit_message>
<xml_diff>
--- a/data/ED/program_details_sample.xlsx
+++ b/data/ED/program_details_sample.xlsx
@@ -731,12 +731,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>School: Edinburgh College of Art | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: Informatics | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Msc Acoustics And Music Technology</t>
+          <t>Msc Advanced Technology For Financial Computing</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -746,44 +746,29 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Taking the science of sound as your focus, you’ll work in a cross-disciplinary environment. You will use theoretical and experimental work to explore the musical, technical and multimedia applications of acoustics and audio technology.
-The emphasis of this programme is on science and technology in the context of musical and multimedia applications.
-The programme aims to:
-provide a broadly based, scientifically-oriented foundation in the area of acoustics, audio, and music technology
-develop your skills in research, computation, design and analytical problem-solving
-give you a strong understanding of music/audio technology
-create a multidisciplinary learning environment that will prepare you for a future career
-You can find more information on the Acoustics and Audio Group website.
-MSc in Acoustics and Music Technology</t>
+          <t>This programme will provide you with a critical and practical appreciation of how data, computing and artificial intelligence technologies can be used and developed. You will learn how this deliver value in organisations with finance, risk and decision-making related digitalisation from both technology and business perspectives.
+The move towards digital organisations offers great potential for small and large, public and private enterprises. Edinburgh is in the UK's second largest financial centre after London and is leading cutting-edge, data-driven innovation to become the data capital of Europe.
+This programme is taught by world class researchers and educators. It is based on full-time cross-disciplinary study and has strong links to existing centres of research excellence within three world-class academic schools within the University:
+School of Informatics
+Edinburgh Business School
+School of Mathematics</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Teaching
-The MSc is taught by a combination of:
-Lectures
-Seminars
-Assessment and dissertation
-Courses are assessed through a combination of report submissions and written examinations.
-In the final three months of the programme, you will carry out an individual project. This is assessed by the submission of a dissertation.</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>- Lectures
- - Seminars
- - Tutorials 
- - practical work</t>
+          <t>This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work. This leads to a dissertation focused on both academic and real-world industry challenges.
+It provides a unique blend of advanced technical courses, including finance-related sectors, and digital business skills with an emphasis on finance elements (minimum 30 credits) from Edinburgh Business School.
+The programme provides you with unique interdisciplinary training. Computing courses build your technical skills. Maths and finance related courses develop your ability to understand the finance system challenges associated with the development, implementation and exploitation of technical solutions.</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=478</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=992</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>two years. In the final three months of the programme, you will carry out an individual project. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+          <t>two years. This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -791,9 +776,14 @@
           <t>9</t>
         </is>
       </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>Academic: total 7.0 with at least 6.0 in each component.</t>
+          <t>总分7.0，小分6</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -803,12 +793,7 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>加分项</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>if you do not meet the academic entry requirements, we may still consider your application if you have professional experience.</t>
+          <t>未要求</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
@@ -845,20 +830,378 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>School: Edinburgh College of Art | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Msc Advanced Sustainable Design</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Advanced Sustainable Design gives you the knowledge, skills and creativity to put theory into practice in the sustainable development of our cities, towns and countryside. We work from the scale of building systems to entire regions.
+We welcome applications from graduates of all disciplines. This programme engages with architecture, design and planning but interested applicants can apply with degrees in the environmental sciences and the humanities.
+Our programme is delivered in a series of practical projects supplemented with teaching on all aspects of built environment sustainable design. You will have the opportunity to work in building simulation modelling and gain desirable skills for the workplace.
+We believe that successful sustainable development is not achieved only through technical solutions. You will:
+explore the complex relationship of design to contemporary sustainable agenda
+engage in cultural and professional debates about the built environment
+gain a distinctive and expert voice in this field
+This programme is affiliated with the University’s Global Environment &amp; Society Academy:
+Global Environment &amp; Society Academy</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>You will complete your studies in one year.
+The first semester is a combination of theory and practice. We will explore the theoretical underpinnings of sustainable design, from a planetary scale to that of a building component.
+Alongside this, you will work on design projects at the scale of both settlements and building systems. We set many of our projects on a global stage, working in a range of climates and contexts.
+The second semester offers an immersive design project that allows you to make your own projects and test them in real contexts.
+You will conclude your studies with a comprehensive dissertation research project that can advance your own interests and be shaped to your preferred career path.</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=417</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>one year. You will complete your studies in one year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>总分6.5，小分6</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>your portfolio should be one, single pdf file of no more than 10 pages. if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>School: Social &amp; Political Science | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Master's Advanced Social Work Studies (mental Health Officer Award) Pgcert</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>This programme is the postgraduate qualification for qualified social workers wishing to practice as mental health officers (MHOs). It has been designed and delivered in partnership with 13 local authorities in the East of Scotland and the University of Edinburgh.
+The programme focuses upon the role of the MHO in relation to relevant Scottish legislation.
+Under Section 32(2) of the Mental Health (Care and Treatment) (Scotland) Act 2003 (the 2003 Act), local authorities have a statutory duty to appoint MHOs to undertake mandatory responsibilities, enshrined in legislation, currently:
+the 2003 Act
+the Adults with Incapacity (Scotland) Act 2000
+the Criminal Procedures (Scotland) Act 1995
+The programme also prepares MHOs to integrate knowledge of other relevant legislation, including:
+the Adult Support and Protection (Scotland) Act 2007
+Its primary aim is to provide the Advanced Social Work Studies (Mental Health Officer Award) in partnership with the East of Scotland MHO Award Partnership.</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>The programme comprises four courses and two practice placements which are taught over one academic year.
+We start with two days induction in mid-October followed by the first course, which begins in late November/December.
+It provides an introduction to some of the key issues and current thinking in the field of mental health and encourages students to take a critical look at subjects and concepts including mental illness, psychiatric diagnoses, recovery and contemporary developments in mental health law.
+The subsequent three courses are structured around the main statutes that frame the MHO role, namely:
+Teaching and learning activities enable students to gain a detailed understanding of this framework and how it interfaces with adult protection legislation.
+The programme benefits from inputs from practising MHOs and allied professionals, including psychiatrists, psychologists and advocacy workers.
+A central focus is the pivotal role MHOs play in navigating the ethical and human rights challenges inherent in this work. This is supported by contributions from people with experience of mental distress and their carers.
+The programme structure enables students to apply their academic learning to real-life situations during the practice placements, supported and supervised by experienced MHOs.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>- The Mental Health (Care and Treatment) (Scotland) Act 2003
+ - The Criminal Procedures (Scotland) Act 1995
+ - The Adults with Incapacity (Scotland) Act 2000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=634</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>two years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. A UK 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>总分7.0，小分6</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>a uk 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice.</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>School: Engineering | College: Science &amp; Engineering</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Msc Advanced Power Engineering</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:
+taught modules
+workshops
+a comprehensive research dissertation carried out during the second year of the programme
+support from the internationally-leading experts of the Institute for Energy Systems
+Our academics regularly lead or participate in large, multi-institutional and multi-national research projects in the area of electrical power engineering. The learning experience is augmented by a number of supporting activities delivered throughout the duration of the programme.
+How will I learn?
+Graduates will be equipped with specialised knowledge associated with the individual modules within the programme. You will develop a deep understanding of advanced power engineering concepts fostered throughout the programme and obtained from the supplementary training activities, study projects and the 2nd year research project.
+The first year of the programme develops from fundamental topics and research tools and techniques in electrical power engineering, to specialist courses on emerging technologies and advanced numerical methods for power engineering problems.
+Research project
+Following the summer break, the second year of the programme is fully dedicated to the Masters research project.
+In close collaboration with academics and researchers of the Institute for Energy Systems, you will put into practice the knowledge and skills acquired during the first year, in application to an actual power engineering problem.
+For the research project there is an option to carry it out within either:
+one of our power research groups, working alongside academics and researchers of the Institute for Energy Systems
+an industrial placement at a collaborating company in the power sector
+Accreditation
+The MSc in Advanced Power Engineering has been accredited by the UK Institution of Engineering and Technology (IET), one the largest professional engineering bodies in the world.
+Your MSc in Advanced Power Engineering can therefore count against the academic requirements for registration as a Chartered Engineer (CEng) in the UK.
+Chartered Engineers not only have a firm grasp of the underpinning knowledge of their field, but also possess the required professional skills to excel in the modern engineering environment.
+Accredited programmes undergo continuous and robust quality review by the IET, and are internationally recognised for their quality of the education they provide.</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>The programme is delivered over 2 years. In Year 1 there are two semesters of taught courses; in Year 2 a research project runs over two semesters leading to the submission of a masters thesis.
+The courses correspond to 120 credits of taught material, plus 120 credits of a research project.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>- Distributed Energy Resources and Smart Grids
+ - Power Engineering Fundamentals 
+ - Power Engineering Laboratory 
+ - Engineering Research Methods with Grand Challenge
+ - Power Systems Engineering and Economics 
+ - Principles of Wind Energy 
+ - Solar Energy &amp; Photovoltaic Systems 
+ - Advanced Power Electronics and Machines 
+ - Research Project: Advanced Power Engineering Dissertation</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=960</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>two-year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. The programme is delivered over 2 years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:.</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>总分6.5，小分6</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>this requirement may be partially met by relevant industrial experience; applicants with non-standard backgrounds may be considered on a case-by-case basis.</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>School: Engineering | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>Msc Advanced Chemical Engineering</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>From carbon capture to sustainable water resources, from alternative energy technologies to advanced pharmaceutical processes, chemical engineers address the frontiers of important global challenges. They formulate and solve today the design problems for the technologies of tomorrow.
 This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields.
@@ -884,7 +1227,7 @@
 The CEng accreditation is awarded by the Institution of Chemical Engineers (IChemE), which is an independent professional body. It gives students and employers confidence in the quality of the MSc Advanced Chemical Engineering programme.</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>In Semester 1, the MSc ACE programme establishes a foundation through compulsory courses which emphasise modern computational techniques and research methods.
 In Semester 2, you will expand your knowledge through a broader selection of optional courses. These focus on:
@@ -897,7 +1240,7 @@
 After the completion of taught modules and confirmation of progression, students focus exclusively on their research project during Semester 3, under the joint supervision of an academic and an industrial partner, with several feedback opportunities.</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>- energy-efficient separation processes
  - multidisciplinary engineering
@@ -934,362 +1277,24 @@
  - Particle Technology Fundamentals and Industrial Applications</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=913</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>one-year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Accreditation of this MSc for CEng (Further Learning) means that our graduates who are seeking to become Chartered Engineers can count their MSc in Advanced Chemical Engineering as one year of Further Learning when applying for the Chartered Engineer status. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields.</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>one-year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields. Accreditation of this MSc for CEng (Further Learning) means that our graduates who are seeking to become Chartered Engineers can count their MSc in Advanced Chemical Engineering as one year of Further Learning when applying for the Chartered Engineer status.</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>The University of Edinburgh</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>爱丁堡大学</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>School: Informatics | College: Science &amp; Engineering</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Msc Advanced Technology For Financial Computing</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>This programme will provide you with a critical and practical appreciation of how data, computing and artificial intelligence technologies can be used and developed. You will learn how this deliver value in organisations with finance, risk and decision-making related digitalisation from both technology and business perspectives.
-The move towards digital organisations offers great potential for small and large, public and private enterprises. Edinburgh is in the UK's second largest financial centre after London and is leading cutting-edge, data-driven innovation to become the data capital of Europe.
-This programme is taught by world class researchers and educators. It is based on full-time cross-disciplinary study and has strong links to existing centres of research excellence within three world-class academic schools within the University:
-School of Informatics
-Edinburgh Business School
-School of Mathematics</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work. This leads to a dissertation focused on both academic and real-world industry challenges.
-It provides a unique blend of advanced technical courses, including finance-related sectors, and digital business skills with an emphasis on finance elements (minimum 30 credits) from Edinburgh Business School.
-The programme provides you with unique interdisciplinary training. Computing courses build your technical skills. Maths and finance related courses develop your ability to understand the finance system challenges associated with the development, implementation and exploitation of technical solutions.</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=992</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work.</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>Academic: total 7.0 with at least 6.5 in each component.</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>The University of Edinburgh</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>爱丁堡大学</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>School: Engineering | College: Science &amp; Engineering</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Msc Advanced Power Engineering</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:
-taught modules
-workshops
-a comprehensive research dissertation carried out during the second year of the programme
-support from the internationally-leading experts of the Institute for Energy Systems
-Our academics regularly lead or participate in large, multi-institutional and multi-national research projects in the area of electrical power engineering. The learning experience is augmented by a number of supporting activities delivered throughout the duration of the programme.
-How will I learn?
-Graduates will be equipped with specialised knowledge associated with the individual modules within the programme. You will develop a deep understanding of advanced power engineering concepts fostered throughout the programme and obtained from the supplementary training activities, study projects and the 2nd year research project.
-The first year of the programme develops from fundamental topics and research tools and techniques in electrical power engineering, to specialist courses on emerging technologies and advanced numerical methods for power engineering problems.
-Research project
-Following the summer break, the second year of the programme is fully dedicated to the Masters research project.
-In close collaboration with academics and researchers of the Institute for Energy Systems, you will put into practice the knowledge and skills acquired during the first year, in application to an actual power engineering problem.
-For the research project there is an option to carry it out within either:
-one of our power research groups, working alongside academics and researchers of the Institute for Energy Systems
-an industrial placement at a collaborating company in the power sector
-Accreditation
-The MSc in Advanced Power Engineering has been accredited by the UK Institution of Engineering and Technology (IET), one the largest professional engineering bodies in the world.
-Your MSc in Advanced Power Engineering can therefore count against the academic requirements for registration as a Chartered Engineer (CEng) in the UK.
-Chartered Engineers not only have a firm grasp of the underpinning knowledge of their field, but also possess the required professional skills to excel in the modern engineering environment.
-Accredited programmes undergo continuous and robust quality review by the IET, and are internationally recognised for their quality of the education they provide.</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>The programme is delivered over 2 years. In Year 1 there are two semesters of taught courses; in Year 2 a research project runs over two semesters leading to the submission of a masters thesis.
-The courses correspond to 120 credits of taught material, plus 120 credits of a research project.</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>- Distributed Energy Resources and Smart Grids
- - Power Engineering Fundamentals 
- - Power Engineering Laboratory 
- - Engineering Research Methods with Grand Challenge
- - Power Systems Engineering and Economics 
- - Principles of Wind Energy 
- - Solar Energy &amp; Photovoltaic Systems 
- - Advanced Power Electronics and Machines 
- - Research Project: Advanced Power Engineering Dissertation</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=960</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>two-year. The programme is delivered over 2 years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>加分项</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>this requirement may be partially met by relevant industrial experience; applicants with non-standard backgrounds may be considered on a case-by-case basis.</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>The University of Edinburgh</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>爱丁堡大学</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>School: Social &amp; Political Science | College: Arts, Humanities &amp; Social Sciences</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Master's Advanced Social Work Studies (mental Health Officer Award) Pgcert</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>This programme is the postgraduate qualification for qualified social workers wishing to practice as mental health officers (MHOs). It has been designed and delivered in partnership with 13 local authorities in the East of Scotland and the University of Edinburgh.
-The programme focuses upon the role of the MHO in relation to relevant Scottish legislation.
-Under Section 32(2) of the Mental Health (Care and Treatment) (Scotland) Act 2003 (the 2003 Act), local authorities have a statutory duty to appoint MHOs to undertake mandatory responsibilities, enshrined in legislation, currently:
-the 2003 Act
-the Adults with Incapacity (Scotland) Act 2000
-the Criminal Procedures (Scotland) Act 1995
-The programme also prepares MHOs to integrate knowledge of other relevant legislation, including:
-the Adult Support and Protection (Scotland) Act 2007
-Its primary aim is to provide the Advanced Social Work Studies (Mental Health Officer Award) in partnership with the East of Scotland MHO Award Partnership.</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>The programme comprises four courses and two practice placements which are taught over one academic year.
-We start with two days induction in mid-October followed by the first course, which begins in late November/December.
-It provides an introduction to some of the key issues and current thinking in the field of mental health and encourages students to take a critical look at subjects and concepts including mental illness, psychiatric diagnoses, recovery and contemporary developments in mental health law.
-The subsequent three courses are structured around the main statutes that frame the MHO role, namely:
-Teaching and learning activities enable students to gain a detailed understanding of this framework and how it interfaces with adult protection legislation.
-The programme benefits from inputs from practising MHOs and allied professionals, including psychiatrists, psychologists and advocacy workers.
-A central focus is the pivotal role MHOs play in navigating the ethical and human rights challenges inherent in this work. This is supported by contributions from people with experience of mental distress and their carers.
-The programme structure enables students to apply their academic learning to real-life situations during the practice placements, supported and supervised by experienced MHOs.</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>- The Mental Health (Care and Treatment) (Scotland) Act 2003
- - The Criminal Procedures (Scotland) Act 1995
- - The Adults with Incapacity (Scotland) Act 2000</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=634</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. A UK 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
-        </is>
-      </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>Academic: total 7.0 with at least 6.0 in each component.</t>
+          <t>总分6.5，小分6</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1299,12 +1304,7 @@
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>需要</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>a uk 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice.</t>
+          <t>未要求</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Msc Advanced Sustainable Design</t>
+          <t>Msc Acoustics And Music Technology</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1356,34 +1356,44 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Advanced Sustainable Design gives you the knowledge, skills and creativity to put theory into practice in the sustainable development of our cities, towns and countryside. We work from the scale of building systems to entire regions.
-We welcome applications from graduates of all disciplines. This programme engages with architecture, design and planning but interested applicants can apply with degrees in the environmental sciences and the humanities.
-Our programme is delivered in a series of practical projects supplemented with teaching on all aspects of built environment sustainable design. You will have the opportunity to work in building simulation modelling and gain desirable skills for the workplace.
-We believe that successful sustainable development is not achieved only through technical solutions. You will:
-explore the complex relationship of design to contemporary sustainable agenda
-engage in cultural and professional debates about the built environment
-gain a distinctive and expert voice in this field
-This programme is affiliated with the University’s Global Environment &amp; Society Academy:
-Global Environment &amp; Society Academy</t>
+          <t>Taking the science of sound as your focus, you’ll work in a cross-disciplinary environment. You will use theoretical and experimental work to explore the musical, technical and multimedia applications of acoustics and audio technology.
+The emphasis of this programme is on science and technology in the context of musical and multimedia applications.
+The programme aims to:
+provide a broadly based, scientifically-oriented foundation in the area of acoustics, audio, and music technology
+develop your skills in research, computation, design and analytical problem-solving
+give you a strong understanding of music/audio technology
+create a multidisciplinary learning environment that will prepare you for a future career
+You can find more information on the Acoustics and Audio Group website.
+MSc in Acoustics and Music Technology</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>You will complete your studies in one year.
-The first semester is a combination of theory and practice. We will explore the theoretical underpinnings of sustainable design, from a planetary scale to that of a building component.
-Alongside this, you will work on design projects at the scale of both settlements and building systems. We set many of our projects on a global stage, working in a range of climates and contexts.
-The second semester offers an immersive design project that allows you to make your own projects and test them in real contexts.
-You will conclude your studies with a comprehensive dissertation research project that can advance your own interests and be shaped to your preferred career path.</t>
+          <t>Teaching
+The MSc is taught by a combination of:
+Lectures
+Seminars
+Assessment and dissertation
+Courses are assessed through a combination of report submissions and written examinations.
+In the final three months of the programme, you will carry out an individual project. This is assessed by the submission of a dissertation.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>- Lectures
+ - Seminars
+ - Tutorials 
+ - practical work</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=417</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=478</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>one year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. You will complete your studies in one year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+          <t>two years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. In the final three months of the programme, you will carry out an individual project. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1391,14 +1401,9 @@
           <t>9</t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
-        </is>
-      </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+          <t>总分7.0，小分6</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
@@ -1413,17 +1418,12 @@
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+          <t>if you do not meet the academic entry requirements, we may still consider your application if you have professional experience.</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>需要</t>
-        </is>
-      </c>
-      <c r="AL7" t="inlineStr">
-        <is>
-          <t>your portfolio should be one, single pdf file of no more than 10 pages. if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+          <t>未要求</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. We encourage you to apply at least one month prior to entry so that we have enough time to process your application.</t>
+          <t>two years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+          <t>总分6.5，小分6</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
@@ -1588,12 +1588,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: Business School | College: Arts, Humanities &amp; Social Sciences</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Msc Online Advanced Nursing (online Learning)</t>
+          <t>Msc Accounting And Finance</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1602,139 +1602,6 @@
         </is>
       </c>
       <c r="M9" t="inlineStr">
-        <is>
-          <t>Our innovative part-time programme offers advanced study for nurses working within an international and UK health care context. 
-We offer the flexibility for you to choose either a broad programme of study by drawing on international expertise across the breadth of the university, or to focus on a more specialised area of nursing care.
-We recognise that mental health and trauma-informed care is an under-developed area in advanced practice for Adult nurses and so we are delighted to offer you the opportunity to choose option courses in these areas, as well as our core courses in nursing and global health policy, political leadership and research. 
-You can choose a range of option courses within Nursing Studies including leadership, public health, policy, person-centred care and clinical decision making. Health and social care research underpin the whole programme.
-The programme is suitable for nurses who are registered to practise in their own country and want to critically examine the ways that evidence-based research, theory and knowledge can advance nursing in the global context. The degree also provides an excellent foundation for postgraduate research e.g. a doctoral degree, or to advance their professional career.</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>This programme offers a flexible online postgraduate degree designed for graduate nurses who are interested in studying at an advanced level.
-The programme is designed to be completed part-time. The minimum period the programme can be completed is two years, with a maximum completion time of three years.
-Students must take two core courses (40 credits) and then can choose from a wide range of option courses offered in semesters 1 and 2 (80 credits). Supervised Reading is also offered in the summer semester (20 credits). In addition, students must complete a dissertation following completion of their taught courses (60 credits). There is a choice of one of two different dissertations – research proposal or e-portfolio.
-For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2. Their dissertation will be completed towards the end of their second year.
-For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. Their dissertation will be completed in year 3.
-The compulsory courses form the core part of the MSc are:
-Optional courses can be chosen from those on offer within the School of Health in Social Science or across the wider university. These vary across years depending on the specific courses on offer, but some of the current nursing online optional courses include:
-We are also delighted to offer a range of option courses with our colleagues in Clinical Psychology and Counselling and Psychological Therapies. 
-This enables you to learn from our team of international experts to inform advanced nursing practice in relation to mental health and trauma-focused health care.
-These option courses include:
-For the latest information available, please see the DRPS.</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>- Nursing and Global Health Policy: developing your political leadership
- - Research Methods in Health
- - Leadership – exploring your potential
- - Global Public Health: a critical approach to health improvement
- - Person Centred Care in Practice: relationships and emotion
- - Supervised Reading
- - Online Counselling Practice and Process
- - Developmental Wellbeing
- - Social Inequality and Child and Adolescent Mental Health
- - Applied Developmental Psychology
- - Trauma and Resilience in a Developmental Context</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=1049</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>two years. MSc Advanced Nursing (Online Learning) (ICL) - 2-6 years (Part-time Intermittent Study) Select your start date 11 September 2023. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. The minimum period the programme can be completed is two years, with a maximum completion time of three years. For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Tuition fees Award Title Duration Study mode   MSc Advanced Nursing Up to 6 Years Part-time Intermittent Study Tuition fees. For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2.</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>Fees for part-time intermittent study
-If you are studying on a part-time intermittent basis then you will be invoiced separately for each course. We refer to this as Invoiced at Course Level (ICL).
-The fees you will pay depend on whether your degree takes place online or on campus.
-Online learning: fees for ICL/intermittent degrees
-On-campus: fees for ICL/intermittent degrees
-Annual tuition fee increase
-Tuition fees increase every year in the majority of cases.
-For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
-From 2023-24 tuition fees for new entrants will be fixed for the duration of their programme. If you joined us from August 2023 onwards and you are studying for a degree or qualification that will take more than one year to complete, the fee charged will be fixed at the level charged on the year of entry.
-Fees and funding
-Work out your fee status
-Find out how and when to pay your tuition fees
-Search for scholarships and funding</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>Academic: total 7.0 with at least 6.5 in each component.</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AI9" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AK9" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>The University of Edinburgh</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>爱丁堡大学</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>School: Business School | College: Arts, Humanities &amp; Social Sciences</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Msc Accounting And Finance</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
         <is>
           <t>Our Accounting and Finance MSc is closely in line with professional practice and is an ideal fit if you are from a quantitative background.
 This is a programme that will challenge you academically, and, through practical applications and case studies, one that will set you up for future roles within Accounting and Finance.
@@ -1746,14 +1613,14 @@
 Bringing together leading academics and practitioners, the centres are a keen theatre of debate, creating new thoughts, new ideas for both the theoretical study and practical application of accounting, finance and investment.</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>Learning will primarily be through:
 Assessment methods include examinations, assignments, presentations or continuous assessment.
 We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>- lectures
  - set reading
@@ -1765,22 +1632,22 @@
  - MSc Accounting and Finance programme structure overview</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=416</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>two years. Tuition fees Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Tuition fees. MSc Accounting and Finance - 1 Year (Full-time) Select your start date 9 September 2024. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Programme structure 2023/24.</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>two years. MSc Accounting and Finance - 1 Year (Full-time) Select your start date 9 September 2024. Tuition fees Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Tuition fees. Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Programme structure 2023/24. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AA10" t="inlineStr">
+      <c r="AA9" t="inlineStr">
         <is>
           <t>Programme fees: Accounting and Finance (MSc)
 Academic Session
@@ -1805,69 +1672,69 @@
 Search for scholarships and funding</t>
         </is>
       </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>Academic: total 7.0 with at least 6.0 in each component.</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AI10" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AK10" t="inlineStr">
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>总分7.0，小分6</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
         <is>
           <t>未要求</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
+    <row r="10">
+      <c r="B10" t="inlineStr">
         <is>
           <t>英国</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>The University of Edinburgh</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>爱丁堡大学</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>22</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>School: Royal (Dick) School of Veterinary Studies | College: Medicine &amp; Veterinary Medicine</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Master's Online Advanced Clinical Practice (online Learning) Pgprofdev</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Veterinary medicine is a rapidly evolving discipline, comprising a wide range of specialist areas. Research in veterinary medicine is directly relevant to the improvement of health and welfare of domestic animal species and the protection of public health.
 Research reputation
@@ -1878,7 +1745,7 @@
 The modular, portfolio approach allows the greatest flexibility to meet the needs of the modern practitioner. The goal is to provide you with the skills and knowledge required to be a highly effective practitioner and to enable you to act as a leader and mentor within the veterinary community.</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci.
 In summary, the completion times are as follows:
@@ -1889,7 +1756,7 @@
 We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>- PgCert: 12-24 months
  - PgDip: 24-48 months
@@ -1897,22 +1764,22 @@
  - More information on PPD</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=910</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>three years. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci. Alternatively, after one year of taking courses you can choose to transfer your credits and continue on to studying towards a higher award on a Masters, Postgraduate Diploma or Postgraduate Certificate programme. The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. Tuition fees Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Tuition fees. PG Professional Development Advanced Clinical Practice (Online Learning) (ICL) - 1-2 Years (Part-time Intermittent Study) Select your start date 11 September 2023 8 January 2024 1 April 2024. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. You may take a maximum of 50 credits worth of courses over two years through our PPD scheme. Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Programme structure 2023/24.</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>three years. Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Programme structure 2023/24. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. You may take a maximum of 50 credits worth of courses over two years through our PPD scheme. Tuition fees Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Tuition fees. Alternatively, after one year of taking courses you can choose to transfer your credits and continue on to studying towards a higher award on a Masters, Postgraduate Diploma or Postgraduate Certificate programme. The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. PG Professional Development Advanced Clinical Practice (Online Learning) (ICL) - 1-2 Years (Part-time Intermittent Study) Select your start date 11 September 2023 8 January 2024 1 April 2024.</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
+      <c r="AA10" t="inlineStr">
         <is>
           <t>If your fees do not display, please check the Tuition Fees website and check your fees by level and year of study.
 Find your tuition fees
@@ -1922,9 +1789,142 @@
 Search for scholarships and funding</t>
         </is>
       </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>总分6.5，小分6</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Msc Online Advanced Nursing (online Learning)</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Our innovative part-time programme offers advanced study for nurses working within an international and UK health care context. 
+We offer the flexibility for you to choose either a broad programme of study by drawing on international expertise across the breadth of the university, or to focus on a more specialised area of nursing care.
+We recognise that mental health and trauma-informed care is an under-developed area in advanced practice for Adult nurses and so we are delighted to offer you the opportunity to choose option courses in these areas, as well as our core courses in nursing and global health policy, political leadership and research. 
+You can choose a range of option courses within Nursing Studies including leadership, public health, policy, person-centred care and clinical decision making. Health and social care research underpin the whole programme.
+The programme is suitable for nurses who are registered to practise in their own country and want to critically examine the ways that evidence-based research, theory and knowledge can advance nursing in the global context. The degree also provides an excellent foundation for postgraduate research e.g. a doctoral degree, or to advance their professional career.</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>This programme offers a flexible online postgraduate degree designed for graduate nurses who are interested in studying at an advanced level.
+The programme is designed to be completed part-time. The minimum period the programme can be completed is two years, with a maximum completion time of three years.
+Students must take two core courses (40 credits) and then can choose from a wide range of option courses offered in semesters 1 and 2 (80 credits). Supervised Reading is also offered in the summer semester (20 credits). In addition, students must complete a dissertation following completion of their taught courses (60 credits). There is a choice of one of two different dissertations – research proposal or e-portfolio.
+For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2. Their dissertation will be completed towards the end of their second year.
+For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. Their dissertation will be completed in year 3.
+The compulsory courses form the core part of the MSc are:
+Optional courses can be chosen from those on offer within the School of Health in Social Science or across the wider university. These vary across years depending on the specific courses on offer, but some of the current nursing online optional courses include:
+We are also delighted to offer a range of option courses with our colleagues in Clinical Psychology and Counselling and Psychological Therapies. 
+This enables you to learn from our team of international experts to inform advanced nursing practice in relation to mental health and trauma-focused health care.
+These option courses include:
+For the latest information available, please see the DRPS.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>- Nursing and Global Health Policy: developing your political leadership
+ - Research Methods in Health
+ - Leadership – exploring your potential
+ - Global Public Health: a critical approach to health improvement
+ - Person Centred Care in Practice: relationships and emotion
+ - Supervised Reading
+ - Online Counselling Practice and Process
+ - Developmental Wellbeing
+ - Social Inequality and Child and Adolescent Mental Health
+ - Applied Developmental Psychology
+ - Trauma and Resilience in a Developmental Context</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=1049</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>two years. For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. MSc Advanced Nursing (Online Learning) (ICL) - 2-6 years (Part-time Intermittent Study) Select your start date 11 September 2023. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Tuition fees Award Title Duration Study mode   MSc Advanced Nursing Up to 6 Years Part-time Intermittent Study Tuition fees. For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2. The minimum period the programme can be completed is two years, with a maximum completion time of three years.</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>Fees for part-time intermittent study
+If you are studying on a part-time intermittent basis then you will be invoiced separately for each course. We refer to this as Invoiced at Course Level (ICL).
+The fees you will pay depend on whether your degree takes place online or on campus.
+Online learning: fees for ICL/intermittent degrees
+On-campus: fees for ICL/intermittent degrees
+Annual tuition fee increase
+Tuition fees increase every year in the majority of cases.
+For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
+From 2023-24 tuition fees for new entrants will be fixed for the duration of their programme. If you joined us from August 2023 onwards and you are studying for a degree or qualification that will take more than one year to complete, the fee charged will be fixed at the level charged on the year of entry.
+Fees and funding
+Work out your fee status
+Find out how and when to pay your tuition fees
+Search for scholarships and funding</t>
+        </is>
+      </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>Academic: total 6.5 with at least 6.0 in each component.</t>
+          <t>总分7.0，小分6</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr">

</xml_diff>

<commit_message>
Feat: ED CN requirement
</commit_message>
<xml_diff>
--- a/data/ED/program_details_sample.xlsx
+++ b/data/ED/program_details_sample.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD11"/>
+  <dimension ref="A1:BD15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,44 +731,84 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>School: Informatics | College: Science &amp; Engineering</t>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Msc Advanced Technology For Financial Computing</t>
+          <t>Master's Msc Ecological Economics</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent. we may also consider a uk 2:2 honours degree, or its international equivalent, with appropriate work experience. applicants from a wide variety of backgrounds are welcome to apply, but all students will be expected to engage critically with economic and environmental concepts, and will also be asked to engage in both quantitative and qualitative analysis. students whose undergraduate degrees have not addressed one or more these areas should highlight in their applications their abilities to learn and to engage with these subject areas. </t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>This programme will provide you with a critical and practical appreciation of how data, computing and artificial intelligence technologies can be used and developed. You will learn how this deliver value in organisations with finance, risk and decision-making related digitalisation from both technology and business perspectives.
-The move towards digital organisations offers great potential for small and large, public and private enterprises. Edinburgh is in the UK's second largest financial centre after London and is leading cutting-edge, data-driven innovation to become the data capital of Europe.
-This programme is taught by world class researchers and educators. It is based on full-time cross-disciplinary study and has strong links to existing centres of research excellence within three world-class academic schools within the University:
-School of Informatics
-Edinburgh Business School
-School of Mathematics</t>
+          <t>From the biodiversity crisis and the climate crisis to the question of managing economies during a global pandemic - the topic of sustainability has never been more pressing.
+The MSc Ecological Economics prepares you to contribute to solving sustainability problems by focusing on the intersection between the environment, the economy and economic decision-making.
+The programme aims to equip you with a new way of seeing the world.  We will empower you to analyse how the economy and economic decisions affect our progress towards a more sustainable future.
+What will I learn?
+The interdisciplinary nature of the programme links environmental, social and economic systems together and focuses on the mutual dependences between them.
+You will participate in sustainability problem-solving with an emphasis on application, practical experience and 'hands-on' learning.
+You will experience training in a wide range of quantitative and qualitative methodologies and the associated data analysis using real-world case studies.
+During your studies, you will implement a small, team-based research project.  Designed collaboratively with staff members in response to a real-world sustainability problem, it will provide you with first-hand experience conducting the work of an ecological economist.
+Scotland’s Rural College
+This programme is delivered in collaboration with Scotland’s Rural College (SRUC).
+You will benefit from being a fully enrolled student at the University of Edinburgh as well as access to all of the complementary staff, expertise, and resources at SRUC.  Upon successful completion of the programme, you will be awarded your degree by the University of Edinburgh.
+Visit the SRUC website
+What’s it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree.  Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work. This leads to a dissertation focused on both academic and real-world industry challenges.
-It provides a unique blend of advanced technical courses, including finance-related sectors, and digital business skills with an emphasis on finance elements (minimum 30 credits) from Edinburgh Business School.
-The programme provides you with unique interdisciplinary training. Computing courses build your technical skills. Maths and finance related courses develop your ability to understand the finance system challenges associated with the development, implementation and exploitation of technical solutions.</t>
+          <t>This MSc programme comprises:
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.  Our courses feature flipped-classroom designs, team-based learning, and problem-based learning. Engagement will happen both in-person and online with both synchronous and asynchronous elements.
+Through this mix of teaching approaches, you will:
+You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+You will build up to completing your dissertation throughout the academic year.
+Part of your preparation will come through compulsory courses (in which you will practice skills you need in the dissertation). Part of your preparation will also come through group and 1:1 sessions that support you in developing and progressing your ideas.  The programme will also help to connect you with potential topics and supervisors.
+Ultimately, this will be your opportunity to explore a topic of your choice in relation to ecological economics and prepare a dissertation that you can use to demonstrate your work to potential employers.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice. Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>- compulsory and option courses
+ - dissertation
+ - learn core conceptual and theoretical knowledge related to ecological economics
+ - gain a wide range of professional and transferable skills
+ - acquire applied knowledge related to research methodologies, data analysis, and project design/implementation. 
+ - Ecological Economics (SAC) (MSc) (Full-time)
+ - Ecological Economics (SAC) (MSc) (Part-time) - 2 years
+ - Ecological Economics (SAC) (MSc) (Part-time) - 3 years</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=992</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=29</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>two years. This MSc consists of approximately seven months of taught courses across two semesters and up to four months of project work. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+          <t>two years. Ecological Economics (SAC) (MSc) (Part-time) - 3 years. Ecological Economics (SAC) (MSc) (Part-time) - 2 years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -778,7 +818,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+          <t>Ecological Economics (SAC) (MSc) Tuition fees; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Ecological+Economics+</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
@@ -793,12 +833,27 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with appropriate work experience.</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>未要求</t>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -830,49 +885,43 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>School: Edinburgh College of Art | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Msc Advanced Sustainable Design</t>
+          <t>Master's Msc Counselling Studies</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, or a uk 2:2 honours degree with a strong personal statement, relevant experience and/or references confirming your aptitude to study at postgraduate level. you should demonstrate a high level of motivation through your personal statement, indicating why you wish to study counselling and demonstrating an understanding of counselling and the capacity to reflect on personal aptitude for work in this field. we may also consider your application if you have professional qualifications equivalent to an honours degree; please contact us to check before you apply. </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Advanced Sustainable Design gives you the knowledge, skills and creativity to put theory into practice in the sustainable development of our cities, towns and countryside. We work from the scale of building systems to entire regions.
-We welcome applications from graduates of all disciplines. This programme engages with architecture, design and planning but interested applicants can apply with degrees in the environmental sciences and the humanities.
-Our programme is delivered in a series of practical projects supplemented with teaching on all aspects of built environment sustainable design. You will have the opportunity to work in building simulation modelling and gain desirable skills for the workplace.
-We believe that successful sustainable development is not achieved only through technical solutions. You will:
-explore the complex relationship of design to contemporary sustainable agenda
-engage in cultural and professional debates about the built environment
-gain a distinctive and expert voice in this field
-This programme is affiliated with the University’s Global Environment &amp; Society Academy:
-Global Environment &amp; Society Academy</t>
+          <t>The programme offers advanced academic study of counselling and related practices. It aims to foster the development of critical reflection on the field by professionally qualified practitioners.
+It complements professional training in counselling by providing students from a range of backgrounds with critical perspectives on counselling and related practices.
+This programme firmly locates the practice of counselling within the field of social science enquiry. Its distinctive features include close links with professional training in counselling and with social science research concerned with counselling and society.
+It includes the professionally validated Postgraduate Certificate in Counselling Studies, three other substantive taught courses and a dissertation based on empirical research.
+This MSc is not a full professional training in counselling. The latter is offered through the Master of Counselling (Interpersonal Dialogue), two years full-time, or the Master of Counselling, four years part-time.</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>You will complete your studies in one year.
-The first semester is a combination of theory and practice. We will explore the theoretical underpinnings of sustainable design, from a planetary scale to that of a building component.
-Alongside this, you will work on design projects at the scale of both settlements and building systems. We set many of our projects on a global stage, working in a range of climates and contexts.
-The second semester offers an immersive design project that allows you to make your own projects and test them in real contexts.
-You will conclude your studies with a comprehensive dissertation research project that can advance your own interests and be shaped to your preferred career path.</t>
+          <t>Teaching and learning methods include lectures, theory seminars and independent study. Assessment is through essays and the dissertation.
+The Postgraduate Certificate component involves experiential group work, practice-skills workshops and individual tutorials, with self and peer assessment and portfolio work, complementing essay-based assessment.
+The programme provides a high level of student-tutor contact and close supervision of both listening practice and research, in line with professional and academic requirements.</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=417</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=131</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>one year. You will complete your studies in one year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+          <t>two years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. The latter is offered through the Master of Counselling (Interpersonal Dialogue), two years full-time, or the Master of Counselling, four years part-time.</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -887,7 +936,7 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>总分6.5，小分6</t>
+          <t>总分7.0，小分6</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
@@ -902,17 +951,22 @@
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+          <t>a uk 2:1 honours degree, or its international equivalent, or a uk 2:2 honours degree with a strong personal statement, relevant experience and/or references confirming your aptitude to study at postgraduate level.</t>
         </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>需要</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>your portfolio should be one, single pdf file of no more than 10 pages. if you do not meet the academic entry requirements, we may still consider your application on the basis of your portfolio and/or relevant professional experience.</t>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -944,59 +998,108 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>School: Social &amp; Political Science | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Master's Advanced Social Work Studies (mental Health Officer Award) Pgcert</t>
+          <t>Management Msc Earth Observation And Geoinformation</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. we also welcome applications from applicants without a degree but who are working as geospatial professionals in the uk armed forces and who have undertaken relevant training. please provide information on any relevant industry experience or training in your personal statement when you apply. </t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>This programme is the postgraduate qualification for qualified social workers wishing to practice as mental health officers (MHOs). It has been designed and delivered in partnership with 13 local authorities in the East of Scotland and the University of Edinburgh.
-The programme focuses upon the role of the MHO in relation to relevant Scottish legislation.
-Under Section 32(2) of the Mental Health (Care and Treatment) (Scotland) Act 2003 (the 2003 Act), local authorities have a statutory duty to appoint MHOs to undertake mandatory responsibilities, enshrined in legislation, currently:
-the 2003 Act
-the Adults with Incapacity (Scotland) Act 2000
-the Criminal Procedures (Scotland) Act 1995
-The programme also prepares MHOs to integrate knowledge of other relevant legislation, including:
-the Adult Support and Protection (Scotland) Act 2007
-Its primary aim is to provide the Advanced Social Work Studies (Mental Health Officer Award) in partnership with the East of Scotland MHO Award Partnership.</t>
+          <t>Combine satellite data, technology and science to find new solutions to the world's biggest challenges.
+The MSc Earth Observation and Geoinformation Management aims to provide you with the theoretical and practical skills to use and analyse Earth observation data in conjunction with broader skills in handling geospatial data.
+This unique programme is well-embedded in an active research and industry environment. It works alongside our successful MSc Geographical Information Science degree, which was the first of its type in the world with a heritage of over 30 years.
+This MSc reflects on the use of geospatial technologies in the detection and mitigation of climate change, sustainability and social responsibility.
+What is Earth Observation and Geoinformation Management?
+Earth observation (EO) involves gathering information about the Earth's physical, chemical, and biological systems using remote sensing technologies such as satellites.
+Earth observation is growing in social, economic and political importance by helping us better understand and manage Earth and its environment in areas such as:
+agriculture
+infrastructure and transportation
+mineral resource management
+land use and planning
+monitoring pollution
+deforestation and land degradation
+climate change monitoring and action
+With Earth observation data and solution delivery now transitioning onto cloud-based service models, it is important to understand the parallel tools in Geographical Information Science (GIS).  In particular, those that support storing, analysing and displaying data related to positions on the Earth's surface to understand spatial patterns and relationships.
+What will I learn?
+Under the guidance of our internationally recognised staff, you will:
+be equipped with critical theoretical knowledge
+develop strong practical skills
+undertake supervised independent research
+We continually refresh the programme to keep you abreast of the latest technologies and anticipate trends and innovative ideas essential in this rapidly growing sector.
+You will gain extensive experience applying Earth observation data 'in the field', including remote sensing. In addition, you will benefit from access to projects that involve the use of equipment such as survey-grade GPS and Unpiloted Aerial Vehicles.
+In addition, you will become part of our unique Edinburgh Earth Observatory Seminar Series. We run these events in association with AGI-Scotland (Association For Geographic Information). The events will enable you to meet a range of professionals and become exposed to new ideas, together with educational and job opportunities.
+Who will teach me?
+Our teaching staff are very research active and benefit from international reputations. We are often invited to engage with other academic institutions, organisations and companies around the world. In addition, we are developing new Earth observation applications and publishing in top tier journals regarding the cryosphere, biosphere and atmosphere.
+We have staff who are part of the science teams for:
+European Space Agency's 'Biomass Mission'
+NASA's GEDI LiDAR on the international space station
+We are also working in international groups to develop the next generation of satellite sensors.
+We also promote a culture of entrepreneurism. For example, several of our staff and former students have set up new Earth observation companies. These companies contribute to Edinburgh's "space ecosystem", which currently includes more than eight space data companies, who can also act as dissertation hosts.
+We are also involved with the Bayes Centre within the University, an international leader in data-driven innovation.
+Our staff are engaged in organisations such as the UK Space Agency and the Intergovernmental Group on Earth Observations (GEO), which shape the UK and worldwide policy on Earth observation. As such, you will learn from experts who have first-hand knowledge of the bigger picture and what is coming next.
+On our website, you can find out how our innovative research in satellite observation and data modelling is making a difference.
+Data-driven research in space and satellites
+Is the MSc for me?
+The program's interdisciplinary nature is ideal if you have a background in environmental or geographical sciences, whether or not you have experience in remote sensing.
+It is also suitable if you have a background in physics, computer science or engineering and looking for a career in more applied areas.
+There is a lot of flexibility in the programme, enabling you to customise your learning in areas you are most passionate about.
+Reputation, relevance and employability
+Our students' research projects are often published in academic or professional journals.
+You will have unrivalled opportunities to connect with Earth observation and GIS professionals, including our alumni network of past graduates, helping you make contacts in the industry.
+Our programme has an excellent reputation amongst employers. In addition, former students will often look first to our graduates when employing new staff. Our alumni network is uniquely active, with alumni regularly contributing to teaching. We also organise an annual conference for alumni, staff and current students. This event often acts as a conduit to employment.  For these reasons, many of our students gain employment by the time they graduate.
+We also maintain close contacts with professional organisations such as The Association for Geographic Information, Royal Institution of Chartered Surveyors and are ideally placed to make connections on your behalf.
+What's it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree.  Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>The programme comprises four courses and two practice placements which are taught over one academic year.
-We start with two days induction in mid-October followed by the first course, which begins in late November/December.
-It provides an introduction to some of the key issues and current thinking in the field of mental health and encourages students to take a critical look at subjects and concepts including mental illness, psychiatric diagnoses, recovery and contemporary developments in mental health law.
-The subsequent three courses are structured around the main statutes that frame the MHO role, namely:
-Teaching and learning activities enable students to gain a detailed understanding of this framework and how it interfaces with adult protection legislation.
-The programme benefits from inputs from practising MHOs and allied professionals, including psychiatrists, psychologists and advocacy workers.
-A central focus is the pivotal role MHOs play in navigating the ethical and human rights challenges inherent in this work. This is supported by contributions from people with experience of mental distress and their carers.
-The programme structure enables students to apply their academic learning to real-life situations during the practice placements, supported and supervised by experienced MHOs.</t>
+          <t>This MSc programme comprises:
+Throughout your studies, we will work with you to prepare you for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to the programme and prepare a dissertation that you can use to demonstrate your work to potential employers.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.  You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice.  Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>- The Mental Health (Care and Treatment) (Scotland) Act 2003
- - The Criminal Procedures (Scotland) Act 1995
- - The Adults with Incapacity (Scotland) Act 2000</t>
+          <t>- compulsory and option courses
+ - dissertation
+ - Earth Observation and Geoinformation Management (MSc) (Full-time)
+ - Earth Observation and Geoinformation Management (MSc) - 2 Years (Part-time)
+ - Earth Observation and Geoinformation Management (MSc) - 3 Years (Part-time)</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=634</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=874</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>two years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. A UK 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+          <t>two years. Earth Observation and Geoinformation Management (MSc) - 3 Years (Part-time). It works alongside our successful MSc Geographical Information Science degree, which was the first of its type in the world with a heritage of over 30 years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Earth Observation and Geoinformation Management (MSc) - 2 Years (Part-time).</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -1006,7 +1109,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+          <t>Earth Observation and Geoinformation Management (MSc) Tuition fees; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Earth+Observation+and+Geoinformation+Management+%28MSc%29</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
@@ -1021,17 +1124,27 @@
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>需要</t>
+          <t>加分项</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>a uk 2:1 honours degree or its international equivalent, or a recognised qualification in social work and at least two years' relevant experience in social work practice.</t>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. please provide information on any relevant industry experience or training in your personal statement when you apply.</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
           <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1063,70 +1176,99 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>School: Engineering | College: Science &amp; Engineering</t>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Msc Advanced Power Engineering</t>
+          <t>Master's Msc Geographical Information Science</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. we also welcome applications from applicants without a degree but who are working as geospatial professionals in the uk armed forces and who have undertaken relevant training. please provide information on any relevant industry experience or training in your personal statement when you apply. </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:
-taught modules
-workshops
-a comprehensive research dissertation carried out during the second year of the programme
-support from the internationally-leading experts of the Institute for Energy Systems
-Our academics regularly lead or participate in large, multi-institutional and multi-national research projects in the area of electrical power engineering. The learning experience is augmented by a number of supporting activities delivered throughout the duration of the programme.
-How will I learn?
-Graduates will be equipped with specialised knowledge associated with the individual modules within the programme. You will develop a deep understanding of advanced power engineering concepts fostered throughout the programme and obtained from the supplementary training activities, study projects and the 2nd year research project.
-The first year of the programme develops from fundamental topics and research tools and techniques in electrical power engineering, to specialist courses on emerging technologies and advanced numerical methods for power engineering problems.
-Research project
-Following the summer break, the second year of the programme is fully dedicated to the Masters research project.
-In close collaboration with academics and researchers of the Institute for Energy Systems, you will put into practice the knowledge and skills acquired during the first year, in application to an actual power engineering problem.
-For the research project there is an option to carry it out within either:
-one of our power research groups, working alongside academics and researchers of the Institute for Energy Systems
-an industrial placement at a collaborating company in the power sector
+          <t>Geographical Information Science (GIS) provides powerful solutions to real-world problems using a range of the world’s most advanced technologies.
+GIS captures, stores, manages and displays data related to positions on the Earth’s surface so you can better understand spatial patterns and relationships.
+Every day around the world, GIS is used to solve complex problems. As a result, it is becoming integrated into almost every discipline.
+From population dynamics, estate planning, logistics management, public health surveillance, and telecommunications to tracking deforestation, environmental management and predicting climate change - GIS is changing the way the world works.
+Always innovative
+Our successful MSc Geographical Information Science was the first of its type in the world.
+It has a heritage of over 30 years and approaching 1000 graduates.  Nevertheless, we continually refresh the programme to keep you abreast of the latest technological changes and industry trends.
+You will gain critical theoretical knowledge, develop strong practical skills and undertake supervised independent research, all under the guidance of our internationally recognised staff.
+In addition, you will become part of our unique Edinburgh Earth Observatory Seminar Series. We run these events in association with AGI-Scotland (Association For Geographic Information). The events will enable you to meet a range of professionals and become exposed to new ideas, together with educational and job opportunities.
+Is the MSc for me?
+This programme reflects on the use of geospatial technologies in the detection and mitigation of climate change, sustainability and social responsibility.
+Our MSc is one of the largest masters programmes in GIS in the world.  We offer foundation courses if you are new to the field and advanced courses if you want to specialise in particular areas.
+You can flexibly choose optional courses to customise your learning in areas you are most passionate about.
+So whether you want to build apps for your smartphone or solve some of the most significant environmental problems on the planet, this programme is for you.
+Reputation, relevance and employability
+A significant number of staff contribute to our programme and benefit from international reputations.  We are often invited to engage with other academic institutions, organisations and companies around the world.
+Our students’ research projects are often published in academic or professional journals.
+Through our alumni network of past graduates, you will have unrivalled opportunities to connect with GIS professionals during your studies, helping you make contacts in the industry. In addition, as part of your dissertation research, options are available to work with various organisations, including the significant ecosystem of companies in Edinburgh, the government and the third sector.
+We maintain close contacts with professional organisations such as The Association for Geographic Information, Royal Institution of Chartered Surveyors and are ideally placed to make connections on your behalf.
+Our programme has an excellent reputation amongst employers. In addition, former students will often look first to our graduates when employing new staff.  Many of our graduates run their own businesses or work at the most senior level in various companies, often contributing to emerging sectors such as data-driven innovation and the green economy.
+Our alumni network is uniquely active, with alumni regularly contributing to teaching.  We also organise an annual conference for alumni, staff and current students. This event often acts as a conduit to employment.  For these reasons, many of our students gain employment by the time they graduate.
+This MSc is the complete package. The variety of the lectures and practicals provided an academic challenge, while the dissertation gave me confidence in the technical aspects, which I really enjoyed. In addition, the University proactively fosters a strong alumni network, meaning another big benefit was realised after the programme had finished with plentiful job opportunities.
+Rob Dunfey, MSc Geographical Information Science
+What’s it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree. Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.
 Accreditation
-The MSc in Advanced Power Engineering has been accredited by the UK Institution of Engineering and Technology (IET), one the largest professional engineering bodies in the world.
-Your MSc in Advanced Power Engineering can therefore count against the academic requirements for registration as a Chartered Engineer (CEng) in the UK.
-Chartered Engineers not only have a firm grasp of the underpinning knowledge of their field, but also possess the required professional skills to excel in the modern engineering environment.
-Accredited programmes undergo continuous and robust quality review by the IET, and are internationally recognised for their quality of the education they provide.</t>
+The MSc Geographical Information Science is accredited by the Royal Institution of Chartered Surveyors (RICS).
+RICS seeks to ensure that graduates have a stimulating and challenging education, preparing them well for their professional careers.
+RICS’s external quality assurance system monitors our curriculum, programme resources, the standard of our graduates and their employability annually to ensure our programme is relevant to industry and maintains professional standards.
+A RICS accredited degree is synonymous with the highest quality of education, benchmarked against international standards, and therefore valued by companies. As RICS’ standards and qualifications are recognised worldwide, it will mean you will hold an internationally recognised qualification.
+If you are considering a career in geomatics or surveying, this accredited degree fast-tracks you towards Chartered status.
+After graduating, you can complete your required Assessment of Professional Competence after just two years of structured workplace training, compared to five years from non-accredited degrees.
+Visit the Royal Institution of Chartered Surveyors website</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>The programme is delivered over 2 years. In Year 1 there are two semesters of taught courses; in Year 2 a research project runs over two semesters leading to the submission of a masters thesis.
-The courses correspond to 120 credits of taught material, plus 120 credits of a research project.</t>
+          <t>This MSc programme comprises:
+You will be taught by leading experts in the field, including both university academics and professional colleagues with many years of experience in GIS.
+You will also have opportunities to attend professional seminars and conferences to understand more about the GIS industry.
+Throughout your studies, we will work with you to prepare you for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to the programme and prepare a dissertation that you can use to demonstrate your work to potential employers.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.
+You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice. Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative. We will continue to update you on the teaching you can expect throughout your application process.</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>- Distributed Energy Resources and Smart Grids
- - Power Engineering Fundamentals 
- - Power Engineering Laboratory 
- - Engineering Research Methods with Grand Challenge
- - Power Systems Engineering and Economics 
- - Principles of Wind Energy 
- - Solar Energy &amp; Photovoltaic Systems 
- - Advanced Power Electronics and Machines 
- - Research Project: Advanced Power Engineering Dissertation</t>
+          <t>- compulsory and option courses
+ - dissertation
+ - Geographical Information Science (MSc) (Full-time)
+ - Geographical Information Science (MSc) (Part-time) - 2 Years
+ - Geographical Information Science (MSc) (Part-time) - 3 Years</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=960</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=74</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>two-year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. The programme is delivered over 2 years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. The two-year MSc programme in Advanced Power Engineering is designed to train power engineers in the most current developments in the field, and help them develop fundamental and applied research skills through a combination of:.</t>
+          <t>two years. Geographical Information Science (MSc) (Part-time) - 2 Years. After graduating, you can complete your required Assessment of Professional Competence after just two years of structured workplace training, compared to five years from non-accredited degrees. It has a heritage of over 30 years and approaching 1000 graduates. Geographical Information Science (MSc) (Part-time) - 3 Years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1134,9 +1276,14 @@
           <t>9</t>
         </is>
       </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Geographical Information Science; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Geographical+Information+Science</t>
+        </is>
+      </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>总分6.5，小分6</t>
+          <t>总分7.0，小分6</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -1151,12 +1298,22 @@
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>this requirement may be partially met by relevant industrial experience; applicants with non-standard backgrounds may be considered on a case-by-case basis.</t>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. please provide information on any relevant industry experience or training in your personal statement when you apply.</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
           <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1188,103 +1345,90 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>School: Engineering | College: Science &amp; Engineering</t>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Msc Advanced Chemical Engineering</t>
+          <t>Management Msc Environmental Protection And</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in biological science, environmental science, physical science, geography, engineering, economics or other relevant subject. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>From carbon capture to sustainable water resources, from alternative energy technologies to advanced pharmaceutical processes, chemical engineers address the frontiers of important global challenges. They formulate and solve today the design problems for the technologies of tomorrow.
-This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields.
-You will learn through:
-taught modules
-coursework
-design projects
-guest lectures
-workshops
-an MSc Research Dissertation
-a number of career supporting activities
-This programme has a particular emphasis on multi-scale approaches and integrated solutions to chemical engineering problems, from the nano-scale to the process scale.
-Learn from industry specialists
-A unique feature of our MSc programme in Advanced Chemical Engineering (ACE) is the strong and committed involvement of the UK and EU chemical engineering industry.
-The programme is advised by an Industrial Advisory Board, and all our MSc Research Dissertation projects are formulated and co-advised by industrial partners, with a wide range of topics including:
-novel processes and materials for carbon capture and storage against climate change
-innovative solutions for energy storage and fuels
-efficient process systems for pharmaceuticals, food and drink manufacturing
-modern concepts and prototypes in healthcare, biomedicine and biotechnology
-Our MSc programme attracts a huge diversity of talent, with 60+ graduates and current students from over 20 countries, spanning four continents. We also work with over 40 industrial partners who help develop and supervise our MSc Research Dissertation projects, ensuring these reflect the latest industry trends and challenges.
+          <t>Your chance to play a vital role to protect and conserve the environment starts here.
+Our actions have had and continue to have a significant impact on our planet:
+the use of natural resources,
+deforestation
+soil erosion
+the release of pollutants and pathogens
+invasive species
+the increase in greenhouse gases
+These human impacts are all examples of pressures that have potentially severe consequences for humanity and other life on Earth.
+The MSc Environmental Protection and Management will give you an in-depth understanding of natural resource management based on a scientific understanding of the issues but also linked across disciplines.
+We will equip you with advanced skills and knowledge about the processes that give rise to environmental degradation and the strategies to affect sustainable change.
+Reputation, relevance and employability
+Our programme has been successfully delivered for over 25 years and continues to grow from strength to strength.
+You will be taught by world-leading experts in key fields, as well as benefiting from our excellent relationships with industry and relevant employers.
+The programme attracts students from a variety of backgrounds.  Our diversity will give you exceptional opportunities to learn from one another and become part of a strong alumni network around the globe.
+Scotland’s Rural College
+This programme is delivered in collaboration with Scotland’s Rural College (SRUC).
+You will benefit from being a fully enrolled student at the University of Edinburgh as well as access to all of the complementary staff, expertise, and resources at SRUC.  Upon successful completion of the programme, you will be awarded your degree by the University of Edinburgh.
+Visit the SRUC website
+What’s it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree. Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.
 Accreditation
-Accreditation of this MSc for CEng (Further Learning) means that our graduates who are seeking to become Chartered Engineers can count their MSc in Advanced Chemical Engineering as one year of Further Learning when applying for the Chartered Engineer status.
-The CEng accreditation is awarded by the Institution of Chemical Engineers (IChemE), which is an independent professional body. It gives students and employers confidence in the quality of the MSc Advanced Chemical Engineering programme.</t>
+The MSc Environmental Protection and Management is accredited by the Institution of Environmental Sciences (IES), allowing students on this programme to become members.
+The IES provides access to news about jobs and events, free journal access and free or reduced entry to IES events.
+Upon completing our MSc programme, you can upgrade for free to become an Associate of the Institution.
+Visit the Institution of Environmental Sciences website</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>In Semester 1, the MSc ACE programme establishes a foundation through compulsory courses which emphasise modern computational techniques and research methods.
-In Semester 2, you will expand your knowledge through a broader selection of optional courses. These focus on:
-A minimum of 10 credits must come from a subset of three Advanced Design optional courses.
-You will have the unique opportunity to:
-Students must select at least one of the next three courses:
-Students can select one of the following courses during Semester 1:
-Plus, between three and six of the following courses (depending on above Advanced Design choices, for a total of 120 credits) during Semester 2:
-The Advanced Chemical Engineering Dissertation (MSc) follows early project allocation and substantial training during Semesters 1-2.
-After the completion of taught modules and confirmation of progression, students focus exclusively on their research project during Semester 3, under the joint supervision of an academic and an industrial partner, with several feedback opportunities.</t>
+          <t>This MSc programme comprises:
+Throughout your studies, we will work with you to prepare you for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to the programme and prepare a dissertation that you can use to demonstrate your work to potential employers.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking. 
+You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.
+Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>- energy-efficient separation processes
- - multidisciplinary engineering
- - management and economics
- - several cutting-edge technological fields
- - learn from leading experts in several fields
- - explore actual industrial processes (with emphasis on design and energy efficiency)
- - acquire technical skills in various areas
- - implement them to actual chemical engineering problems
- - hone your communication and human skills to present your original achievements
- - Numerical Methods for Chemical Engineers
- - Molecular Thermodynamics 
- - Introduction to Research Methods 
- - Advanced Chemical Engineering Dissertation
- - Separation Processes for Carbon Capture (Semester 2)
- - Oil and Gas Systems Engineering (Semester 2)
- - Group Design Project (Advanced Chemical Engineering Design) (Semester 2)
- - Chemical Reaction Engineering 
- - Fire Science and Fire Dynamics
- - Engineering Project Management 
- - Supply Chain Management  
- - Technology and Innovation Management 
- - Technology Entrepreneurship
- - Adsorption
- - Gas Separations Using Membranes 
- - Separation Processes
- - Advanced Process Safety
- - Batchwise and Semibatch Processing 
- - Bio-Inspired Engineering 
- - Biotechnology and Bioprocess Engineering
- - Polymer Science and Engineering
- - Nanomaterials in Chemical and Biomedical Engineering 
- - Electrochemical Engineering 
- - Particle Technology Fundamentals and Industrial Applications</t>
+          <t>- compulsory and option courses
+ - dissertation
+ - Environmental Protection and Management (MSc) (Part-time) - 2 Years
+ - Environmental Protection and Management (MSc) (Part-time) - 3 Years
+ - Environmental Protection and Management (MSc) - 1 Year (Full-time)</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=913</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=31</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>one-year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. This one-year MSc programme at the University of Edinburgh will immerse you in cutting-edge developments in these and many more multidisciplinary fields. Accreditation of this MSc for CEng (Further Learning) means that our graduates who are seeking to become Chartered Engineers can count their MSc in Advanced Chemical Engineering as one year of Further Learning when applying for the Chartered Engineer status.</t>
+          <t>two years. Environmental Protection and Management (MSc) (Part-time) - 2 Years. Environmental Protection and Management (MSc) (Part-time) - 3 Years. Environmental Protection and Management (MSc) - 1 Year (Full-time). Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Reputation, relevance and employability Our programme has been successfully delivered for over 25 years and continues to grow from strength to strength.</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1292,9 +1436,14 @@
           <t>9</t>
         </is>
       </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>Environmental Protection and Management (MSC) Tuition fees; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Environmental+protection+and+management</t>
+        </is>
+      </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>总分6.5，小分6</t>
+          <t>总分7.0，小分6</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1304,12 +1453,27 @@
       </c>
       <c r="AI6" t="inlineStr">
         <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience.</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>未要求</t>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1341,59 +1505,91 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>School: Edinburgh College of Art | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Msc Acoustics And Music Technology</t>
+          <t>Management Msc Carbon</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in a relevant subject such as environmental sciences, management, social sciences, energy, sustainability, earth sciences, physical sciences, geology, geography, economics, biology, health sciences, engineering, business administration, or finance. we may also consider degrees in other disciplines if you can demonstrate how it is relevant to the programme, or if you have relevant work experience in a related field. we may also consider a uk 2:2 honours degree, or its international equivalent, if you have substantial, related professional experience. please provide information on any relevant experience in your personal statement when you apply. </t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Taking the science of sound as your focus, you’ll work in a cross-disciplinary environment. You will use theoretical and experimental work to explore the musical, technical and multimedia applications of acoustics and audio technology.
-The emphasis of this programme is on science and technology in the context of musical and multimedia applications.
-The programme aims to:
-provide a broadly based, scientifically-oriented foundation in the area of acoustics, audio, and music technology
-develop your skills in research, computation, design and analytical problem-solving
-give you a strong understanding of music/audio technology
-create a multidisciplinary learning environment that will prepare you for a future career
-You can find more information on the Acoustics and Audio Group website.
-MSc in Acoustics and Music Technology</t>
+          <t>Are you ready to confront the challenges of the global climate crisis?
+Join students from across the globe to tackle the challenges of climate change and create a low-carbon economy.
+With our MSc Carbon Management, you will have the opportunity to develop the skills and knowledge to engage critically with climate change debates and challenges for an equitable transition toward a resilient, low-carbon future.
+This interdisciplinary programme is fast-paced and dynamic.  Your studies will draw widely on the latest research in the climate change field, plus case studies from Scotland and worldwide.
+Industry experts, including alumni of the programme, also contribute to the discussions and provide guest lectures.
+Throughout this interactive degree, you are encouraged to dive in and join the conversation, participate in group activities, and offer your critical analysis of the topics. Together, we work to create a culture of positivity in how we think about and act towards the global climate crisis challenge.
+Is the MSc for me?
+If you want a career where you can be part of the solution to one of the world’s greatest and most complex challenges, this programme is for you.
+The MSc Carbon Management is designed for a diverse range of graduates from the natural, environmental and social sciences, as well as from business, economics, management studies and other related degrees who are passionate about combatting climate change.
+We are also looking for people that want to be entrepreneurs in the climate change field.
+Edinburgh Climate Change Institute
+The MSc Carbon Management is associated with the Edinburgh Climate Change Institute (ECCI).
+ECCI brings together law, business, social science, technology, and policy experts to help develop a low-carbon society.
+Through ECCI, you will have the opportunity to work and network alongside professionals and potential employers within this high-demand field.
+Visit the Edinburgh Climate Change Institute website
+What’s it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+MSc Climate Change Finance and Investment
+Please note that this programme is not a substitute for the MSc Climate Change Finance and Investment. If you are keen to focus your studies on carbon finance and investment, we encourage you to find out more details and apply to the Business School.
+MSc Climate Change Finance and Investment
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+on the right panel of this page.
+You should also avoid applying to more than one degree.  Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.
+Accreditation
+This programme is accredited by the Institute of Environmental Management &amp; Assessment (IEMA).
+IEMA is the global professional body for individuals and organisations working in environment and sustainability.  A programme accredited by the IEMA ensures that graduates leaving environmental programmes have the right knowledge, skills and tools to deliver value in a global economy. Students enrolled on an IEMA approved are equipped with the expertise and understanding they need to secure a job in environment and sustainability and ultimately, lead change.
+Students enrolled in our MSc Carbon Management are eligible for free IEMA Student Membership, underpinning their studies with an invaluable toolkit of resources.
+Visit the IEMA website
+(Revised 9 February 2023 to add in accreditation information)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Teaching
-The MSc is taught by a combination of:
-Lectures
-Seminars
-Assessment and dissertation
-Courses are assessed through a combination of report submissions and written examinations.
-In the final three months of the programme, you will carry out an individual project. This is assessed by the submission of a dissertation.</t>
+          <t>This MSc programme comprises:
+You will be taught various topics and themes across the required courses, including climate science, climate change risk, mitigation and adaptation, economics, policy, business, and climate justice.
+Throughout the programme, your teaching team will work with you to prepare for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to climate change and carbon management. You can even use the dissertation to explore your own business idea for tackling climate change through the business plan dissertation option.
+We also work with our wide network to find opportunities for dissertation projects with external organisations, enhancing the real-world relevance of your degree.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.
+You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice.  Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.
+(Revised 19 July 2023 to remove ‘Climate Change Economics’ from the compulsory courses for the 2023/24 academic year.)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>- Lectures
- - Seminars
- - Tutorials 
- - practical work</t>
+          <t>- compulsory and option courses
+ - dissertation
+ - Carbon Management (MSc)
+ - Carbon Management (MSc) - 2 Years (Part-time)
+ - Carbon Management (MSc) - 3 Years (Part-time)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=478</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=412</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>two years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. In the final three months of the programme, you will carry out an individual project. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+          <t>two years. Carbon Management (MSc) - 2 Years (Part-time). Carbon Management (MSc) - 3 Years (Part-time). Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1401,6 +1597,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>Carbon Management (MSc) Tuition fees; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Carbon+Management+%28MSC%29</t>
+        </is>
+      </c>
       <c r="AC7" t="inlineStr">
         <is>
           <t>总分7.0，小分6</t>
@@ -1418,12 +1619,22 @@
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>if you do not meet the academic entry requirements, we may still consider your application if you have professional experience.</t>
+          <t>we may also consider degrees in other disciplines if you can demonstrate how it is relevant to the programme, or if you have relevant work experience in a related field.</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
           <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1455,78 +1666,60 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>School: Health in Social Science | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: Chemistry | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Msc Advanced Nursing</t>
+          <t>Master's Msc Medicinal And Biological Chemistry</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in chemistry, or a closely related discipline, with a strong chemistry component. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience and supportive references. </t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>This innovative programme offers advanced study for nurses working within a global context to enhance practice at the local level.
-You can either choose a specific pathway: leadership, clinical research* or education, or follow a flexible generic programme with the opportunity to study a range of relevant courses from across the School of Health in Social Science and the wider University.
-Nursing, health and social care research underpins the whole programme.
-You will begin the MSc at the same entry point as all other students, but depending on the pathway you would like to undertake, have the opportunity to exit with a range of different degree titles:
-MSc Advanced Nursing
-MSc Advanced Nursing (leadership)
-MSc Advanced Nursing (education)
-MSc Advanced Nursing (clinical research)
-Who is this programme for?
-The programme is suitable if you are a nurse registered in any branch of the profession to practice in your own country and you want to critically examine the ways that evidence-based research, theory and knowledge can advance nursing in the global context.
-The degree also provides an excellent foundation for postgraduate research e.g. a doctoral degree, or to advance their professional career.
-*The clinical research pathway is only available for students who are registered with the Nursing Midwifery Council in the UK to practice in a clinical setting.</t>
+          <t>In this MSc in Medicinal and Biological Chemistry, you will explore the role of biomolecules in life, disease and biotechnology from a chemical perspective.
+You will gain a thorough understanding of the structures, properties, functions, applications and manipulation of biological molecules, from macromolecules to cells, whilst also discussing the design of exciting new medicines in the laboratory and their function in clinical settings. This also requires the chemical understanding of synthetic molecules, their structures, properties, analysis and synthesis.
+The programme will have a strong practical element and significant continuous assessment. This includes a practical research project, which provides you with invaluable experience of working on a real research project on a medicinal or biological chemistry topic.
+Much of the teaching is designed specifically for the MSc students and you will be assessed through a combination of:
+coursework
+laboratory reports
+presentations
+exams
+performance and reporting on the MSc research project
+The knowledge and skills acquired in the programme will leave graduates well equipped to compete for positions in chemical, pharmaceutical or biotechnology companies.
+The lecture courses include topics in:
+Concepts in Medicinal and Biological Chemistry
+Advanced Medicinal Chemistry
+Advanced Biological Chemistry
+Optional Courses in Chemistry
+Laboratory Techniques and Research Techniques
+These are studied concurrently with a predominantly practical based course offering an introduction to research methods related to medicinal and biological chemistry.
+Students then proceed to a period of full-time research project work, leading to the submission of their Masters dissertation.
+MSc Student Experience</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Teaching is delivered in a range of engaging and interactive formats by academic and specialist staff working in the contemporary health care environment.
-Teaching methods include:
-As a full-time MSc student, you will take two core courses and two option courses each semester.
-There is a choice of one of three different dissertations:
-This is to be completed during the Semester 3.
-You can follow one of three different pathways: leadership, education or clinical research, or can take a generic pathway, depending on career aspirations and areas of interest.
-As a part-time student, you can choose one or two courses each semester and have a choice of dissertation in your final year.
-You can also follow the three different pathways or take a generic pathway.
-The compulsory courses form the core part of the MSc and are:
-You can then choose 4 optional taught courses before you go on to undertake the dissertation.
-Optional courses can be chosen from those on offer within the School of Health in Social Science or across the wider University and are dependent on the pathway that the student chooses.
-Optional courses vary across years depending on the specific courses on offer, but some of the current optional courses available include:</t>
+          <t>Lectures are given by leading researchers in the area of medicinal and biological chemistry.
+The lecture courses are supported by tutorial sessions and assessed by coursework and examination.
+The MSc programme provides experience and training in activities that are important to professional chemists and to the research process, such as:</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>- lectures
- - seminars
- - workshops
- - tutor-led online learning environments
- - empirical
- - research proposal
- - e-portfolio
- - Global Leadership in Nursing: Policy, Informatics and Innovation
- - Designing research in Nursing, Health and Social care
- - Clinical Decision Making and Professional Judgement
-Teaching Practice Attachment
- - Leadership - exploring your potential (distance)
- - Global Public Health: a critical approach to health improvement
- - Conducting Research in Nursing, Health and Social care
- - Health Research Methods workshops
- - Homeless and Inclusion Health
- - Cancer Care
- - Transplant nursing
- - Community nursing
- - Person Centred Care in Practice: Relationships and Emotion</t>
+          <t>- science communication
+ - data handling and statistics 
+ - modern laboratory techniques in Chemistry
+ - relevant transferable skills</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=419</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=450</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1539,6 +1732,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
+        </is>
+      </c>
       <c r="AC8" t="inlineStr">
         <is>
           <t>总分6.5，小分6</t>
@@ -1551,12 +1749,27 @@
       </c>
       <c r="AI8" t="inlineStr">
         <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience and supportive references.</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AK8" t="inlineStr">
-        <is>
-          <t>未要求</t>
+      <c r="AO8" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP8" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1588,58 +1801,98 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>School: Business School | College: Arts, Humanities &amp; Social Sciences</t>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Msc Accounting And Finance</t>
+          <t>Master's Msc Soils And Sustainability</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in biological science, environmental science, physical science, geography, engineering, economics or other relevant subject. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Our Accounting and Finance MSc is closely in line with professional practice and is an ideal fit if you are from a quantitative background.
-This is a programme that will challenge you academically, and, through practical applications and case studies, one that will set you up for future roles within Accounting and Finance.
-Industry connections
-Studying accounting and finance in Edinburgh will give you the opportunity to be based at the heart of the UK's second largest financial centre. Many of Europe's leading financial institutions have their headquarters here, a fact that we make full use of on the MSc programme.
-We regularly bring guest speakers to the School to talk directly to Accounting and Finance students on real, current practice.
-The School also maintains good relationships with a number of accounting and finance professionals who will be on hand to provide advice on research and career opportunities. Essential connections like these characterise the dynamic nature of this programme.
-Our strong connection to industry is exemplified by our work in the Centre for Financial Markets Research, and the Institute of Public Sector Accounting Research.
-Bringing together leading academics and practitioners, the centres are a keen theatre of debate, creating new thoughts, new ideas for both the theoretical study and practical application of accounting, finance and investment.</t>
+          <t>Soil systems are a vital resource.
+They provide multiple ecosystem services and are an essential component of food production and food security globally.
+Soils can act as both a net sink and net source of atmospheric carbon dioxide. Therefore, soils play a crucial role in climate change regulation, which has gained increasing international attention in recent years.
+Our MSc Soils and Sustainability is an interdisciplinary programme, providing you with the essential knowledge and advanced skills to make informed decisions on sustainable land practice.
+The programme encompasses the fundamentals of soil science and soil's role in wider environmental systems, sustainable land management, and monitoring techniques to evaluate soils' role and effective management in various environmental landscapes and socioeconomic contexts.
+The need for sustainable soil systems
+Did you know it takes up to 1,000 years to produce just 2-3cm of soil?
+Yet the United Nations report that the equivalent of one football field of soil is eroded every 5 seconds. Over 33% of the Earth's soils are already degraded.
+Therefore, with a rapidly increasing global population and the threat of climate change, sustainable soil systems will play a vital role in future food security.  They are under increasing attention to contribute to climate regulation through carbon sequestration.
+Soils and sustainable land use are vital in terms of providing important habitats to support biodiversity. In addition, soils can contribute to flood regulation and buffer pollutant transfers to local watercourses influencing water quality through effective management.  Soil environments also provide foundations for infrastructure and cultural heritage.
+What will I learn?
+The MSc will prepare you for a range of careers in land-based management and environmental protection.
+You will explore:
+Soil formation, functions and ecosystem services
+Role of soils in mitigating climate change
+Soil health and causes of degradation
+Management strategies to promote and conserve soil health and sustainable soil systems
+Practical skills in soil analysis and surveying
+You will learn to interpret data and information on soil physics, biology and chemistry for the preservation and maintenance of soil health and gain a greater understanding of soil biodiversity, ecology and ecosystem services, as well as global-scale issues and threats to soil systems.
+The programme places a strong emphasis on varied teaching approaches for both theoretical understanding and practical skills, such as laboratory and field-based activities.
+Reputation, relevance and employability
+The MSc is delivered by world-renowned experts and researchers across a range of disciplines within the soil and environmental sciences.
+You will learn from our academic staff and guest lecturers, who are experts in their respective fields.
+This means you will benefit from the most up-to-date research-led knowledge on soils and sustainability, as well as links to other organisations and industries.
+During your dissertation project, you will be encouraged to engage and collaborate with a wide network such as government bodies, conservation organisations and consultants.
+Not only will this provide you with opportunities to expand your network for employment opportunities or research projects, but also help enhance your knowledge and skillset with valuable real-world experience.
+Scotland's Rural College
+This programme is delivered in collaboration with Scotland's Rural College (SRUC).
+You will benefit from being a fully enrolled student at the University of Edinburgh as well as access to all of the complementary staff, expertise, and resources at SRUC.  Upon successful completion of the programme, you will be awarded your degree by the University of Edinburgh.
+Visit the SRUC website
+What's it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree. Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Learning will primarily be through:
-Assessment methods include examinations, assignments, presentations or continuous assessment.
-We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+          <t>This MSc programme comprises:
+Your teaching team will work with you throughout the programme to help prepare and develop your dissertation project. This will be your opportunity to explore a topic of your choice, which will be designed specifically to develop your skill set in relation to your individual interests and career goals.
+For example, your bespoke project can be developed from your own idea and/or in collaboration with external organisations and/or with current ongoing research conducted at SRUC and the University of Edinburgh.
+Your dissertation can incorporate desk- and practical-based skills and methodologies used within the wide-ranging field of sustainable land management that underpin environmental protection, food security and climate change issues that directly relate to current employment opportunities.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.
+You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice.  Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative. We will continue to update you on the teaching you can expect throughout your application process.</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>- lectures
- - set reading
- - class discussions
- - exercises
- - group-work assignments
- - problem-solving in tutorials 
- - case studies
- - MSc Accounting and Finance programme structure overview</t>
+          <t>- compulsory and option courses
+ - dissertation
+ - Soils and Sustainability (MSc) (Full-time)
+ - Soils and Sustainability (MSc) (Part-time) - 2 years
+ - Soils and Sustainability (MSc) (Part-time) - 3 years</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=416</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=781</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>two years. MSc Accounting and Finance - 1 Year (Full-time) Select your start date 9 September 2024. Tuition fees Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Tuition fees. Award Title Duration Study mode   MSc Accounting and Finance 1 Year Full-time Programme structure 2023/24. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+          <t>two years. After 30 years in business, I was becoming very concerned about the environment. The need for sustainable soil systems Did you know it takes up to 1,000 years to produce just 2-3cm of soil? Yet the United Nations report that the equivalent of one football field of soil is eroded every 5 seconds. Soils and Sustainability (MSc) (Part-time) - 2 years. Soils and Sustainability (MSc) (Part-time) - 3 years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1649,27 +1902,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>Programme fees: Accounting and Finance (MSc)
-Academic Session
-Scotland
-Rest of
-UK
-International/
-EU
-Online Distance Learning
-Additional Programme Costs
-2024/5
-Home fees have still to be agreed
-Home fees have still to be agreed
-£39,500.00
-Annual tuition fee increase
-Tuition fees increase every year in the majority of cases.
-For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
-From 2023-24 tuition fees for new entrants will be fixed for the duration of their programme. If you joined us from August 2023 onwards and you are studying for a degree or qualification that will take more than one year to complete, the fee charged will be fixed at the level charged on the year of entry.
-Fees and funding
-Work out your fee status
-Find out how and when to pay your tuition fees
-Search for scholarships and funding</t>
+          <t>Soils and Sustainability (MSc) Tuition fees; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=soils+and+sustainability</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
@@ -1684,12 +1917,27 @@
       </c>
       <c r="AI9" t="inlineStr">
         <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience.</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AK9" t="inlineStr">
-        <is>
-          <t>未要求</t>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP9" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1721,57 +1969,62 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>School: Royal (Dick) School of Veterinary Studies | College: Medicine &amp; Veterinary Medicine</t>
+          <t>School: Chemistry | College: Science &amp; Engineering</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Master's Online Advanced Clinical Practice (online Learning) Pgprofdev</t>
+          <t>Master's Msc Materials Chemistry</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in chemistry or a closely related discipline with a strong chemistry component e.g. chemical engineering or materials science. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience and supportive references. applicants should have a strong chemistry background with at least three continuous years of chemistry subjects throughout their degree. we may accept fewer chemistry courses if applicants have a strong science background e.g. mathematics/physics. applicants should also have completed a minimum of first year university level mathematics, e.g. calculus or linear algebra. </t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Veterinary medicine is a rapidly evolving discipline, comprising a wide range of specialist areas. Research in veterinary medicine is directly relevant to the improvement of health and welfare of domestic animal species and the protection of public health.
-Research reputation
-The R(D)SVS has an international reputation, and its clinical services - Hospital for Small Animals (dog and cat and exotics, zoo and wildlife) and Large Animal Hospital (equine and livestock) - are among the most influential centres for clinical care in the UK and Europe. It is best placed to advance the skills of the sector due to the skills in primary, secondary and tertiary care medicine and surgery, and its extensive research activities in all aspects of veterinary medicine.
-Who is this programme for?
-Veterinary practitioners are under pressure to maintain high standards of practice while also keeping abreast of the latest developments. In response to the increasing requirement for support in developing advanced clinical skills, this distance learning programme is aimed primarily, but not exclusively, at veterinarians in practice.
-How will I learn?
-The modular, portfolio approach allows the greatest flexibility to meet the needs of the modern practitioner. The goal is to provide you with the skills and knowledge required to be a highly effective practitioner and to enable you to act as a leader and mentor within the veterinary community.</t>
+          <t>Materials Chemistry has emerged as an important sub-discipline within Chemistry. It cross-cuts the traditional organic/inorganic/physical boundaries of Chemistry and overlaps many disciplines from Engineering to the Biosciences.
+Materials chemists now have a leading role in areas such as:
+microelectronics
+polymer science
+catalysis
+nanotechnology
+They also make an important contribution to areas of more traditional chemistry such as the pharmaceutical sector.
+Here, understanding the 'physical properties' of intermediates and products is now recognised as essential in optimising the synthesis and properties of pharmaceutically active ingredients in medicines.
+The degree consists of advanced lecture courses such as:
+Concepts of Materials Chemistry
+Advanced Materials Chemistry
+Optional Courses in Chemistry
+Advanced Analytical and Characterisation Methods
+Laboratory Techniques
+These are studied concurrently with a predominantly practical based course offering an introduction to laboratory techniques and research methods pertinent to materials chemistry.
+Students then proceed to a period of full-time research project work leading to the submission of their Master's dissertation.
+MSc Student Experience</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci.
-In summary, the completion times are as follows:
-The programme is modular in structure, offering a flexible student-centred approach to the choice of courses studied. You can choose to take a particular species track in the elective course, i.e. courses focussed on companion animals, exotic zoo and wildlife, equine or production animals. Equally, you can choose to take a mixed-practice approach by selecting courses that meet your individual professional needs.
-Each year will consist of three 11-week terms structured into two blocks of five weeks of study with a week in between for independent study and reflection. One block of five weeks will equate to 10 credits of course material. This framework is designed to fit in with the part-time nature of the programme, giving you time to reflect on your learning and lessening the impact of the additional requirements that studying will place on your working life.
-Postgraduate Professional Development (PPD) is aimed at working professionals who want to advance their knowledge through a postgraduate-level course(s), without the time or financial commitment of a full Masters, Postgraduate Diploma or Postgraduate Certificate.
-You may take a maximum of 50 credits worth of courses over two years through our PPD scheme. These lead to a University of Edinburgh postgraduate award of academic credit. Alternatively, after one year of taking courses you can choose to transfer your credits and continue on to studying towards a higher award on a Masters, Postgraduate Diploma or Postgraduate Certificate programme. Although PPD courses have various start dates throughout a year you may only start a Masters, Postgraduate Diploma or Postgraduate Certificate programme in the month of September. Any time spent studying PPD will be deducted from the amount of time you will have left to complete a Masters, Postgraduate Diploma or Postgraduate Certificate programme.
-We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+          <t>Lectures are given by leading researchers in the area of materials chemistry. The lecture courses are supported by tutorial sessions, and assessed by coursework and examination.
+The MSc programme also provides experience and training in activities that are important to professional chemists and to the research process, such as:</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>- PgCert: 12-24 months
- - PgDip: 24-48 months
- - MVetSci: 36-72 months
- - More information on PPD</t>
+          <t>- science communication
+ - data handling and statistics 
+ - modern laboratory techniques in Chemistry
+ - various other transferable skills</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=910</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=448</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>three years. Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Programme structure 2023/24. You may undertake the programme by intermittent study (flexible progression route), accruing credits within a maximum time limit of two years for the Postgraduate Certificate, four years for the Postgraduate Diploma and six years for the MVetSci. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. You may take a maximum of 50 credits worth of courses over two years through our PPD scheme. Tuition fees Award Title Duration Study mode   PgProfDev Advanced Clinical Practice Up to 2 Years Part-time Intermittent Study Tuition fees. Alternatively, after one year of taking courses you can choose to transfer your credits and continue on to studying towards a higher award on a Masters, Postgraduate Diploma or Postgraduate Certificate programme. The programme is delivered part-time by online learning over a minimum period of three years and a maximum period of six years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. PG Professional Development Advanced Clinical Practice (Online Learning) (ICL) - 1-2 Years (Part-time Intermittent Study) Select your start date 11 September 2023 8 January 2024 1 April 2024.</t>
+          <t>two years. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
@@ -1781,12 +2034,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>If your fees do not display, please check the Tuition Fees website and check your fees by level and year of study.
-Find your tuition fees
-Fees and funding
-Work out your fee status
-Find out how and when to pay your tuition fees
-Search for scholarships and funding</t>
+          <t>信息不可用 Tuition Fees/fees找不到，也没有项目专用的学费链接</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
@@ -1801,12 +2049,27 @@
       </c>
       <c r="AI10" t="inlineStr">
         <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience and supportive references.</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AK10" t="inlineStr">
-        <is>
-          <t>未要求</t>
+      <c r="AO10" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP10" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>
@@ -1843,61 +2106,57 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Msc Online Advanced Nursing (online Learning)</t>
+          <t>Master's Mcouns Counselling (interpersonal Dialogue)-2023不开放申请</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in a subject relevant to counselling and psychotherapy. you should also have substantial relevant experience of working in helping roles in counselling or a cognate area, such as education, social work, nursing, mental health practice, applied psychology or equivalent. we will also consider a uk 2:2 honours degree, or its international equivalent, in a subject relevant to counselling and psychotherapy with references confirming your aptitude for study at postgraduate level. if your undergraduate degree is not relevant to counselling and psychotherapy, you may be admitted at the discretion of the programme director as long as you meet the personal and professional suitability and relevant experience requirements laid down by the british professional bodies for counselling and psychotherapy. check the programme website for more information: entry is subject to passing a professional suitability interview. as this is a professional training programme, students are subject to the university's fitness to practise policies and processes. </t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Our innovative part-time programme offers advanced study for nurses working within an international and UK health care context. 
-We offer the flexibility for you to choose either a broad programme of study by drawing on international expertise across the breadth of the university, or to focus on a more specialised area of nursing care.
-We recognise that mental health and trauma-informed care is an under-developed area in advanced practice for Adult nurses and so we are delighted to offer you the opportunity to choose option courses in these areas, as well as our core courses in nursing and global health policy, political leadership and research. 
-You can choose a range of option courses within Nursing Studies including leadership, public health, policy, person-centred care and clinical decision making. Health and social care research underpin the whole programme.
-The programme is suitable for nurses who are registered to practise in their own country and want to critically examine the ways that evidence-based research, theory and knowledge can advance nursing in the global context. The degree also provides an excellent foundation for postgraduate research e.g. a doctoral degree, or to advance their professional career.</t>
+          <t>This programme is a two year, full-time professionally validated postgraduate qualification in counselling. It is an accelerated version of the well-established Master of Counselling (MCouns), which is offered over four years part-time.
+The programme is specifically designed for international students, with significant (one to two years) professional experience in related fields, who are seeking to gain a fully accredited professional qualification in counselling in the
+United Kingdom. This programme is also open to UK students with significant professional experience.
+Combining academic rigour with high quality professional training, the programme provides unique opportunities for training, learning and research in the field of counselling and psychotherapy.
+The award of this degree qualifies graduates to practise as counsellors or therapists in the UK and in other countries with equivalent professional and academic standards.
+The programme is founded in dialogue between the person-centred approach and psychodynamic perspectives in counselling. It involves substantial placement practice (in unpaid internships) with counselling clients.
+Entry is subject to passing a professional suitability interview.  As this is a professional training programme, students are subject to the University's Fitness to Practise policies and processes.</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>This programme offers a flexible online postgraduate degree designed for graduate nurses who are interested in studying at an advanced level.
-The programme is designed to be completed part-time. The minimum period the programme can be completed is two years, with a maximum completion time of three years.
-Students must take two core courses (40 credits) and then can choose from a wide range of option courses offered in semesters 1 and 2 (80 credits). Supervised Reading is also offered in the summer semester (20 credits). In addition, students must complete a dissertation following completion of their taught courses (60 credits). There is a choice of one of two different dissertations – research proposal or e-portfolio.
-For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2. Their dissertation will be completed towards the end of their second year.
-For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. Their dissertation will be completed in year 3.
-The compulsory courses form the core part of the MSc are:
-Optional courses can be chosen from those on offer within the School of Health in Social Science or across the wider university. These vary across years depending on the specific courses on offer, but some of the current nursing online optional courses include:
-We are also delighted to offer a range of option courses with our colleagues in Clinical Psychology and Counselling and Psychological Therapies. 
-This enables you to learn from our team of international experts to inform advanced nursing practice in relation to mental health and trauma-focused health care.
-These option courses include:
-For the latest information available, please see the DRPS.</t>
+          <t>You will be taught through:
+Your assessments will include:
+The programme provides a high level of student-tutor contact and close supervision of both counselling practice and research, in line with professional and academic requirements.</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>- Nursing and Global Health Policy: developing your political leadership
- - Research Methods in Health
- - Leadership – exploring your potential
- - Global Public Health: a critical approach to health improvement
- - Person Centred Care in Practice: relationships and emotion
- - Supervised Reading
- - Online Counselling Practice and Process
- - Developmental Wellbeing
- - Social Inequality and Child and Adolescent Mental Health
- - Applied Developmental Psychology
- - Trauma and Resilience in a Developmental Context</t>
+          <t>- experiential group work
+ - counselling practice
+ - supervision of counselling practice
+ - theory seminars
+ - independent study
+ - mentorship 
+ - academic support
+ - essays
+ - seminar presentations
+ - self and peer assessments
+ - placement-based assessment
+ - the professional portfolio 
+ - a dissertation (for relevant programmes)</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=1049</t>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=520</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>two years. For students undertaking the 3 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 40 credits are completed in year one and the reminder in year 2 and/or year 3. MSc Advanced Nursing (Online Learning) (ICL) - 2-6 years (Part-time Intermittent Study) Select your start date 11 September 2023. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Tuition fees Award Title Duration Study mode   MSc Advanced Nursing Up to 6 Years Part-time Intermittent Study Tuition fees. For students undertaking the 2 year programme, they will usually take one or two 20 credit courses each semester, so that a minimum of 60 credits are completed in year one and the remainder in year 2. The minimum period the programme can be completed is two years, with a maximum completion time of three years.</t>
+          <t>two year. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. The programme is specifically designed for international students, with significant (one to two years) professional experience in related fields, who are seeking to gain a fully accredited professional qualification in counselling in the. This programme is a two year, full-time professionally validated postgraduate qualification in counselling. It is an accelerated version of the well-established Master of Counselling (MCouns), which is offered over four years part-time.</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -1905,23 +2164,6 @@
           <t>9</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>Fees for part-time intermittent study
-If you are studying on a part-time intermittent basis then you will be invoiced separately for each course. We refer to this as Invoiced at Course Level (ICL).
-The fees you will pay depend on whether your degree takes place online or on campus.
-Online learning: fees for ICL/intermittent degrees
-On-campus: fees for ICL/intermittent degrees
-Annual tuition fee increase
-Tuition fees increase every year in the majority of cases.
-For students whose studies commenced in 2022-23 or earlier, tuition fees will increase each year. You should take this annual tuition fee increase into consideration when you estimate your fees for a degree.
-From 2023-24 tuition fees for new entrants will be fixed for the duration of their programme. If you joined us from August 2023 onwards and you are studying for a degree or qualification that will take more than one year to complete, the fee charged will be fixed at the level charged on the year of entry.
-Fees and funding
-Work out your fee status
-Find out how and when to pay your tuition fees
-Search for scholarships and funding</t>
-        </is>
-      </c>
       <c r="AC11" t="inlineStr">
         <is>
           <t>总分7.0，小分6</t>
@@ -1929,17 +2171,710 @@
       </c>
       <c r="AG11" t="inlineStr">
         <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>entry is subject to passing a professional suitability interview. check the programme website for more information: entry is subject to passing a professional suitability interview.</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>you should also have substantial relevant experience of working in helping roles in counselling or a cognate area, such as education, social work, nursing, mental health practice, applied psychology or equivalent. if your undergraduate degree is not relevant to counselling and psychotherapy, you may be admitted at the discretion of the programme director as long as you meet the personal and professional suitability and relevant experience requirements laid down by the british professional bodies for counselling and psychotherapy.</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AI11" t="inlineStr">
+      <c r="AO11" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP11" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Master's Msc Environment, Culture And Society</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience. </t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>The MSc Environment, Culture and Society provides up-to-date knowledge of the contemporary issues and debates on the relationships between the environment, nature, culture and society.
+Welcoming students from a variety of backgrounds, this exciting MSc will explore the core perspectives, concepts, and practices from the arts, humanities and social sciences needed to imagine and enact sustainable environmental futures.
+You will develop the critical and creative skills and abilities to assess the importance and implications of geographical and other conceptual debates which shape environmental policy and practice.
+Reputation and relevance
+Taught by world-leading experts, the programme draws on expertise from across the University, especially from:
+geography
+social and political studies
+landscape architecture
+literature
+archaeology
+philosophy
+theology
+science and technology studies
+development studies
+It provides you with a unique critical and creative perspective on current environmental issues and possible futures.
+You will learn to think critically, engage creatively and generate new knowledge related to the environment.  In addition, you will be able to use this knowledge effectively to address urgent environmental challenges across a range of specialities such as policy, conservation, education, public consultation and the arts.
+Is the MSc for me?
+The programme's interdisciplinary nature is ideal if you have a background in environmental humanities, social sciences, or creative arts.
+It is also suitable if you desire to understand the roots of our current environmental emergency and the possibilities for a better future.
+There is a lot of flexibility in the programme, enabling you to customise your learning in areas you are most passionate about. For example, philosophy, policy, creative practice and political action.
+Networks
+This programme is affiliated with a variety of University networks, including:
+School of GeoSciences Cultural and Historical Geography Research Group
+Global Environment and Society Academy
+Energy and Society Network
+Edinburgh Environmental Humanities Network
+What's it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+on the right panel of this page.
+You should also avoid applying to more than one degree. Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>This MSc programme comprises:
+Throughout your studies, we will work with you to prepare you for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to the programme and prepare a dissertation that you can use to demonstrate your work to potential employers.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.  You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice. Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>- compulsory and option courses
+ - dissertation
+ - Environment, Culture and Society (MSc) (Full-time)
+ - Environment, Culture and Society (MSc) (Part-time) - 2 Years</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=395</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>two years. Environment, Culture and Society (MSc) (Part-time) - 2 Years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>[Environment, Culture and Society (MSc) Tuition fees](; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Environment%2C+Culture+and+Society+%28MSc%29; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Environment%2C+Culture+and+Society+%28MSc%29; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Environment%2C+Culture+and+Society+%28MSc%29&lt;/a&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>总分7.0，小分6</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
         <is>
           <t>未要求</t>
         </is>
       </c>
-      <c r="AK11" t="inlineStr">
+      <c r="AI12" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ12" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant industry experience.</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
         <is>
           <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO12" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP12" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Master's Msc Energy, Society And Sustainability</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience, a strong personal statement and supportive reference. </t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>How do we achieve energy security, energy justice and environmental sustainability across different contexts, timescales, places and people?
+This question we all face is the ‘energy trilemma’.
+With the MSc Energy, Society and Sustainability, you can explore these challenges affecting our world today and in the future.
+Energy - at the heart of sustainability
+Energy comes in many forms. First, its availability in the landscape, such as coal, wind or the sun, must be transformed into electricity. It is then carried in pipes and grids to where it is needed to power our everyday lives.
+All this takes materials and has an economic, environmental and human cost. Yet, energy is essential to everyday human life and at the heart of sustainability. To address global climate change, the world needs a fast but fair transition to a low-carbon society.
+Scotland and Edinburgh are prime contexts in which to investigate such dynamics. Scotland is a world leader in renewable electricity generation. It has a history of hydroelectricity and North Sea oil and a future in tide and wave energy.  However, it also has high levels of energy poverty, a challenge faced by many.
+What will I learn?
+The MSc in Energy, Society and Sustainability equips you with an understanding of how different societies can address the challenge of balancing energy with sustainability. It brings together a social, political, economic, and environmental understanding of low-carbon technologies.
+You will explore the risks, costs, and benefits of transitioning to low-carbon energy in a globalised world.
+The programme will equip you with a critical awareness of related local, regional and global debates and challenges, such as the United Nations Sustainable Development Goals and the role of energy in development.
+You will benefit from our access to insightful case studies, as well as the organisations and communities our lecturers work closely with, from local Scottish islands to international corporations.  These cases demonstrate global best practices and identify paths to sustainable energy management.
+Reputation, relevance and employability
+You will be taught by experts and researchers, many of whom are leaders in their field.
+We are also committed to helping you benefit from our excellent relationships.  We engage with government departments, energy-relevant NGOs, and key industry players from community energy organisations to start-up renewable energy companies.
+These networks provide opportunities for you to meet potential employers and for dissertations conducted in partnership with external organisations, helping you gain valuable real-world experience.
+Is the MSc for me?
+We welcome students from a wide range of backgrounds, creating a unique opportunity for interdisciplinary shared learning.
+Students with a natural science background might seek to understand the social factors associated with a lower carbon economy.  Social science students might expand their skills and knowledge for a career in low-carbon energy.
+Edinburgh Climate Change Institute
+The MSc Carbon Management is associated with the Edinburgh Climate Change Institute (ECCI).  ECCI brings together law, business, social science, technology, and policy experts to help develop a low-carbon society.
+Through ECCI, you will have the opportunity to work and network alongside professionals and potential employers within this high-demand field.
+Visit the Edinburgh Climate Change Institute website
+What’s it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree. Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>This MSc programme comprises:
+Throughout your studies, we will work with you to prepare you for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to the programme and prepare a dissertation that you can use to demonstrate your work to potential employers.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.  You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice.  Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>- compulsory and option courses
+ - dissertation
+ - Energy, Society and Sustainability (MSc) - 1 Year (Full-time)
+ - Energy, Society and Sustainability (MSc) - 2 Years (Part-time)</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2022&amp;id=934</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>two years. Energy, Society and Sustainability (MSc) - 2 Years (Part-time). Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old. Energy, Society and Sustainability (MSc) - 1 Year (Full-time).</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>总分7.0，小分6</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience, a strong personal statement and supportive reference.</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO13" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP13" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>School: Edinburgh Medical School: Biomedical Sciences | College: Medicine &amp; Veterinary Medicine</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Master's Msc Human Anatomy</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent, in a medical, biomedical or relevant bioscience subject, or other subject allied to medicine. we may also consider applicants with a uk 2:1 or 2:2 honours degree or its international equivalent, if you have other qualifications with relevant work experience, normally of at least one year; for example if you have human anatomy work experience (i.e. human anatomy tutor, demonstrator, dissector etc) or in medical and paramedical fields. please contact the programme team to check before you apply. </t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>This 12-month programme offers a rare opportunity to learn anatomy from dissection and experience in teaching human anatomy. This is an ideal stepping-stone to a career in anatomy teaching and research.
+With this highly regarded qualification you will gain major transferable skills through an intensive on-campus dissection course and develop teaching experience at undergraduate and postgraduate level.
+What will you study?
+This programme has two main strands.
+Develop your in-depth knowledge of human anatomy through dissection
+Anatomical knowledge will be learned to a level to teach undergraduate and postgraduate students and professions allied to medicine. This strand will involve the dissection of a body in groups of three to five students over two semesters. This part of the course is largely self-directed, with regular “surgeries” when teaching staff are present to answer questions and help students with the dissections.
+Learn to teach anatomy
+The second strand is anatomy teaching, covering the theoretical and practical aspects of teaching anatomy to undergraduate and postgraduate students. Alongside theoretical lectures and workshops in the first semester, you will focus on observing the teaching of anatomy to medical undergraduate students.
+In the second semester you will be involved in preparing and carrying out teaching sessions to both small and large groups of students. You will compile an end-of-year teaching portfolio based on:
+the theoretical material you learn
+the observations you make
+the practical experience you have gained
+the experience that you will gain can be used towards an application as associate fellow of the Higher Education Academy
+Embryology course
+Complementing these strands will be a lecture-based embryology course. This will provide you with an understanding of normal human development and how normal development can go wrong, manifested in commonly observed congenital abnormalities.
+You will also study:
+Neuroanatomy
+Embryology
+Anatomy law and ethics
+Medical imaging
+The health and safety of embalming procedures and handling bodies
+The legal and historical aspects of anatomy in Scotland and the UK
+An introduction to the ethics of using bodies in medical education</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>The programme is made up of five courses plus a summer dissertation project.
+The courses Basic Human Anatomy, Imaging, Embryology 1 and Basic Human Anatomy, Imaging, Embryology 2 make up the majority of the degree with 40 credits each.
+The teaching anatomy course is 20 credits whereas the other courses are 10 credit courses that are spread out over two semesters as follows (10 credits equal 100 hours of work):
+Basic Human Anatomy, Imaging and Embryology 1 (40 credits): Provides students with an in-depth knowledge of the anatomy of the upper/lower limbs and thorax, incorporating:
+Anatomy Law and Ethics (10 credits): Divided into 3 parts:
+Basic Human Anatomy, Imaging and Embryology 2 (40 credits): Provides students with an in-depth knowledge of the anatomy of the abdomen, pelvis and head and neck, incorporating:
+Neuroanatomy (10 credits): Gross anatomy of the:
+Teaching is by lectures, seminars and tutorials.
+Courses are assessed by either, or a combination of:
+You have the option to finish after the second semester graduating with a Diploma in Human Anatomy, or to gain your masters by completing a summer dissertation project that can be either library-, practical- or laboratory-based.
+More information on anatomy at the University can be found on our website:</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>- Basic Human Anatomy, Imaging and Embryology 1 (40 credits): Provides students with an in-depth knowledge of the anatomy of the upper/lower limbs and thorax, incorporating:
+gross anatomy
+surface anatomy
+medical imaging 
+embryology
+ - gross anatomy
+ - surface anatomy
+ - medical imaging 
+ - embryology
+ - Anatomy Law and Ethics (10 credits): Divided into 3 parts:
+health and safety of anatomy and body handling
+the legislation that governs the activities of anatomy departments both in Scotland and throughout the UK
+the ethics of using human material for the teaching of anatomy
+ - health and safety of anatomy and body handling
+ - the legislation that governs the activities of anatomy departments both in Scotland and throughout the UK
+ - the ethics of using human material for the teaching of anatomy
+ - Basic Human Anatomy, Imaging and Embryology 2 (40 credits): Provides students with an in-depth knowledge of the anatomy of the abdomen, pelvis and head and neck, incorporating:
+gross anatomy
+surface anatomy
+medical imaging 
+embryology
+ - gross anatomy
+ - surface anatomy
+ - medical imaging 
+ - embryology
+ - Neuroanatomy (10 credits): Gross anatomy of the:
+central and peripheral nervous systems
+sensory and motor pathways
+cranial nerves
+spinal cord
+spinal nerves 
+autonomic nervous system
+ - central and peripheral nervous systems
+ - sensory and motor pathways
+ - cranial nerves
+ - spinal cord
+ - spinal nerves 
+ - autonomic nervous system
+ - Teaching Anatomy (20 credits): Theoretical and practical aspects of teaching anatomy to undergraduate and postgraduate students
+ - Dissertation Project: 10,000 word dissertation and oral presentation (60 credits)
+ - oral examinations
+ - essays
+ - multiple choice question exams
+ - extended matching question exams
+ - presentations 
+ - practical anatomy exams
+ - Anatomy at Edinburgh</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=648</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>one year. This 12-month programme offers a rare opportunity to learn anatomy from dissection and experience in teaching human anatomy. We may also consider applicants with a UK 2:1 or 2:2 honours degree or its international equivalent, if you have other qualifications with relevant work experience, normally of at least one year. We encourage you to apply at least one month prior to entry so that we have enough time to process your application. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>总分6.5，小分6</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI14" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>we may also consider applicants with a uk 2:1 or 2:2 honours degree or its international equivalent, if you have other qualifications with relevant work experience, normally of at least one year; for example if you have human anatomy work experience (i.e.</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO14" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP14" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>The University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>爱丁堡大学</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>School: GeoSciences | College: Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Master's Msc Environment And Development</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">these entry requirements are for the 2023/24 academic year and requirements for future academic years may differ. entry requirements for the 2024/25 academic year will be published on 2 october 2023. a uk 2:1 honours degree, or its international equivalent. we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience, a strong personal statement and supportive reference. </t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Are you ready to explore some of the world's most pressing challenges?
+Understand the link between the environment and development agendas and global inequalities - for today and the future.
+The MSc Environment and Development enables you to critically evaluate the multiple dimensions of the inter-relationship between development and the environment, with an abiding concern for social and environmental justice.
+What will I learn?
+You will learn about issues that are inherently transboundary, multi-generational and multi-faceted, such as:
+sustainable development
+climate change
+diminishing natural resources
+biodiversity conservation
+water
+food
+'waste'
+energy
+disaster risk
+vulnerability and adaptation
+gender and social equality
+urbanisation
+Attempts to understand and address these interconnected issues need to pay close attention to their contested, political and ideological nature.
+That is why our MSc foregrounds society and nature as inherently linked, historical contexts as highly relevant to current debates, and global capitalism as an underlying force of change.
+Issues will be explored across a range of geographical scales, seeing the local and global as necessarily inter-related.
+It will consider the increasingly diverse set of actors, practices and processes driving environment and development issues, and question the power of these to direct agendas and actions.
+The MSc has relevance in both the 'Global South' and 'Global North', drawing attention to relationships of inequality and marginalisation as they occur for particular environments and sections of society worldwide.
+It will provide you with a unique critical perspective, as it draws on expertise from across the University, especially from development geography, social and political sciences, and environmental studies.
+You can explore society and environment issues through different theoretical and conceptual lenses, examining the interplay of sociocultural perspectives, economics and governance, development debates and ecological dynamics.
+There is much diversity in what you can study and conduct research on.  Our flexibility enables you to develop your interests at an advanced level in an area you are most passionate about.
+How will I learn?
+Our teaching approach encourages you to reflect upon your own role, as both researchers and as professionals, in transformations towards social and environmental justice, considering the ethics of engagement in an unequal world.
+The programme helps you develop:
+critical reflective skills
+strong research and critical analysis capabilities
+professional skills tailored to environment and development sectors
+a deep understanding of social and environmental issues
+It provides a strong basis for engaged citizenship in the world, enabling you to contribute to world debates and actions for reducing inequalities and working towards social and environmental justice and more sustainable practices.
+Reputation, relevance and employability
+You will be taught by world-leading researchers and experienced practitioners working in environment and development fields in various sectors from non-government organisations (NGOs), consultancies, or state organisations.
+Guest speakers and teaching staff will provide insights into real-world applications.
+We will challenge you to cultivate reflective research thinking that is cross-cutting and globally relevant.
+This programme is affiliated with the University's Global Development Academy.
+Is the MSc for me?
+The MSc Environment Development will suit a range of students, including those who have practical experience in the broad field of environment and development, either as practitioners, volunteers or activists.
+It is suitable for students from a wide range of undergraduate disciplines, from the environmental and natural sciences to the social and political sciences and humanities.
+We are fortunate to attract a wide range of students from around the world, and we celebrate that diversity and the opportunities for learning that it brings.
+What's it really like to study here?
+Visit our blog, where students in the School of GeoSciences share their experiences of postgraduate study, living in Edinburgh and everything in-between.
+Student experience blog
+When to apply
+Please note: Due to high demand for this programme, we operate on a series of early application deadlines
+.
+We strongly recommend you apply as early as possible.
+For dates and details, please refer to
+'Application Deadlines'
+and
+'How to apply'
+on the right panel of this page.
+You should also avoid applying to more than one degree. Applicants who can demonstrate their understanding and commitment to a specific programme are preferred.
+If you plan to apply to more than one programme, you should discuss your choices with us before you submit your application.
+Where possible, we may make an alternative programme offer if you have been unsuccessful in your chosen programme.</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>This MSc programme comprises:
+Throughout your studies, we will work with you to prepare you for the dissertation project. This will be your opportunity to explore a topic of your choice in relation to the programme and prepare a dissertation that you can use to demonstrate your work to potential employers.
+As we are committed to helping people into education while continuing to work or managing family and personal commitments, you may study this programme part-time.
+You will experience a range of learning styles while studying, depending on the subject matter and courses you are taking.
+You can view each relevant course for teaching and assessment methods through the ‘Programme Structure’ link under compulsory and option courses below.
+Although we endeavour to provide a wide range of optional courses to choose from, these can be subject to change or cancellation at short notice.  Places on optional courses can be limited due to course capacity and timetabling constraints. It may not be possible to guarantee every offer holder their top choice of optional courses.
+We link to the latest information available. Please note that this may be for a previous academic year and should be considered indicative.</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>- compulsory and option courses
+ - dissertation
+ - Environment and Development (MSc) (Full-time)
+ - Environment and Development (MSc) (Part-time) - 2 Years
+ - Environment and Development (MSc) (Part-time) - 3 Years</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>https://www.ed.ac.uk/studying/postgraduate/degrees/index.php?r=site/view&amp;edition=2023&amp;id=30</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>two years. Environment and Development (MSc) (Part-time) - 2 Years. Environment and Development (MSc) (Part-time) - 3 Years. Your English language qualification must be no more than three and a half years old from the start date of the programme you are applying to study, unless you are using  , TOEFL, Trinity   or  , in which case it must be no more than two years old.</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>Environment and Development (MSc) Tuition fees; https://www.ed.ac.uk/tuition-fees/find/postgraduate-taught/2023-2024/taught-masters?keyword=Environment+and+Development+%28MSc%29+</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>总分7.0，小分6</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AI15" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>we may also consider a uk 2:2 honours degree, or its international equivalent, with relevant work experience, a strong personal statement and supportive reference.</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AO15" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AP15" t="inlineStr">
+        <is>
+          <t>有条件2:2</t>
         </is>
       </c>
     </row>

</xml_diff>